<commit_message>
Added sheet "Parameters" in Template
Also appended (NOT USED IN CURRENT VERSION) to Scaling factor for infection hospitalisation rate.
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8A3A64-DF29-3043-9347-8C6F0558EC0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6E9271-46FE-0B40-BCAA-49E86F518634}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="23740" windowHeight="15780" tabRatio="648" activeTab="7" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="7280" yWindow="460" windowWidth="20700" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Cases" sheetId="2" r:id="rId2"/>
     <sheet name="Severity-Mortality" sheetId="4" r:id="rId3"/>
     <sheet name="Population" sheetId="3" r:id="rId4"/>
-    <sheet name="Country Area Parameters" sheetId="7" r:id="rId5"/>
-    <sheet name="Virus Parameters" sheetId="8" r:id="rId6"/>
-    <sheet name="Hospitalisation Parameters" sheetId="9" r:id="rId7"/>
-    <sheet name="Interventions" sheetId="11" r:id="rId8"/>
-    <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId9"/>
+    <sheet name="Parameters" sheetId="13" r:id="rId5"/>
+    <sheet name="Country Area Parameters" sheetId="7" r:id="rId6"/>
+    <sheet name="Virus Parameters" sheetId="8" r:id="rId7"/>
+    <sheet name="Hospitalisation Parameters" sheetId="9" r:id="rId8"/>
+    <sheet name="Interventions" sheetId="11" r:id="rId9"/>
+    <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Interventions!$A$1:$H$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Interventions!$A$1:$H$65</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,35 +39,43 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
     <author>Olivier Celhay</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{2EE5D9F9-70D2-4739-AFAE-0614035B39C6}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{0CC5576C-A1A7-7841-B0C3-592EE60CFC15}">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-0 - 100%</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 to 0.2</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{75449A71-E16D-874C-A4E3-E802E681943C}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{2764A438-DFDE-924B-A542-066F81FC1E24}">
       <text>
         <r>
           <rPr>
@@ -95,11 +104,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 to 7 days</t>
+          <t>0 to 100</t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="1" shapeId="0" xr:uid="{000E9CFB-1FDB-EE47-B9BF-8F8DB282F20A}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{8AD2806A-0360-764B-88F6-A679E1DACDA3}">
       <text>
         <r>
           <rPr>
@@ -128,59 +137,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 to 7 days</t>
+          <t>0 to 100</t>
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{B9D281D5-26D2-4EA9-8894-5FF5A286FE33}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-1 - 12 (Jan - Dec)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{F5DB51BD-EBA9-4F27-8D31-176034A1BBB8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{2040E543-4D10-1848-9CA9-2D20FF237DBA}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{E23ECAEF-C282-A74D-A2C9-55CAD5E28C7F}">
       <text>
         <r>
           <rPr>
@@ -209,7 +170,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>0.5 to 150 years</t>
+          <t>0 to 100</t>
         </r>
       </text>
     </comment>
@@ -224,7 +185,7 @@
     <author>Olivier Celhay</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{19EEFD16-A4C8-43F7-B777-1E668FAB69A6}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{2EE5D9F9-70D2-4739-AFAE-0614035B39C6}">
       <text>
         <r>
           <rPr>
@@ -232,7 +193,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -241,14 +202,80 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{24739DE5-5B28-428F-A3AB-933649284A03}">
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{75449A71-E16D-874C-A4E3-E802E681943C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 7 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="1" shapeId="0" xr:uid="{000E9CFB-1FDB-EE47-B9BF-8F8DB282F20A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 7 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{B9D281D5-26D2-4EA9-8894-5FF5A286FE33}">
       <text>
         <r>
           <rPr>
@@ -256,7 +283,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -265,14 +292,38 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 - 4</t>
+1 - 12 (Jan - Dec)</t>
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="1" shapeId="0" xr:uid="{3FD13DF3-4955-2247-AAA2-68EC3599CA31}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{F5DB51BD-EBA9-4F27-8D31-176034A1BBB8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{2040E543-4D10-1848-9CA9-2D20FF237DBA}">
       <text>
         <r>
           <rPr>
@@ -301,172 +352,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="1" shapeId="0" xr:uid="{96AD9494-0E73-EB4D-B4E7-5944E1089063}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="1" shapeId="0" xr:uid="{6AF90CD2-69CC-AA4B-A769-14DADD96C490}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{15100A51-88F1-2D4A-BE13-B9EA8C6490CE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{5813D783-EA21-DD45-B6C5-56D42BCEDA80}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="1" shapeId="0" xr:uid="{0F7FC5C6-6ECF-DF4D-84D6-9F029454BE66}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
+          <t>0.5 to 150 years</t>
         </r>
       </text>
     </comment>
@@ -477,6 +363,239 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Author</author>
+    <author>Olivier Celhay</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{19EEFD16-A4C8-43F7-B777-1E668FAB69A6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="1" shapeId="0" xr:uid="{3FD13DF3-4955-2247-AAA2-68EC3599CA31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="1" shapeId="0" xr:uid="{96AD9494-0E73-EB4D-B4E7-5944E1089063}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="1" shapeId="0" xr:uid="{6AF90CD2-69CC-AA4B-A769-14DADD96C490}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{15100A51-88F1-2D4A-BE13-B9EA8C6490CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{5813D783-EA21-DD45-B6C5-56D42BCEDA80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="1" shapeId="0" xr:uid="{0F7FC5C6-6ECF-DF4D-84D6-9F029454BE66}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 30 days</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>Olivier Celhay</author>
     <author>Author</author>
   </authors>
@@ -635,7 +754,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -644,7 +763,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -659,7 +778,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -668,7 +787,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -683,7 +802,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -692,7 +811,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -741,7 +860,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -750,7 +869,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 1 - 5</t>
@@ -765,7 +884,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -774,7 +893,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 1 - 10</t>
@@ -834,7 +953,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -843,7 +962,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -858,7 +977,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -867,7 +986,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -927,7 +1046,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -936,7 +1055,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -996,7 +1115,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1005,7 +1124,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1020,7 +1139,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1029,7 +1148,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1044,7 +1163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1053,7 +1172,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1113,7 +1232,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1122,7 +1241,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1137,7 +1256,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1146,7 +1265,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1195,7 +1314,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1204,7 +1323,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1219,7 +1338,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1228,7 +1347,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1310,7 +1429,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1319,7 +1438,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1412,7 +1531,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1421,7 +1540,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1469,7 +1588,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1478,7 +1597,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1493,7 +1612,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1502,7 +1621,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1562,7 +1681,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1571,7 +1690,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1586,7 +1705,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -1595,7 +1714,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 0 - 100%</t>
@@ -1607,7 +1726,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="247">
   <si>
     <t>date</t>
   </si>
@@ -2239,67 +2358,115 @@
     <t>Deaths per person per day</t>
   </si>
   <si>
-    <t>Template v12</t>
-  </si>
-  <si>
-    <t>Scaling factor for infection hospitalisation rate:</t>
+    <t>Screening/Overdispersion:</t>
+  </si>
+  <si>
+    <t>Screening/Contacts:</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>screen_overdispersion</t>
+  </si>
+  <si>
+    <t>screen_contacts</t>
+  </si>
+  <si>
+    <t>Days to implement maximum quarantine coverage:</t>
+  </si>
+  <si>
+    <t>quarantine_effort</t>
+  </si>
+  <si>
+    <t>Duration of hospitalised infection:</t>
+  </si>
+  <si>
+    <t>Duration of denied hospitalisation infection:</t>
+  </si>
+  <si>
+    <t>Duration of ICU infection:</t>
+  </si>
+  <si>
+    <t>Duration of denied ICU infection:</t>
+  </si>
+  <si>
+    <t>Duration of ventilated infection:</t>
+  </si>
+  <si>
+    <t>Duration of denied ventilation infection:</t>
+  </si>
+  <si>
+    <t>Age-based relative fatality rate in well-resourced scenario (%)</t>
+  </si>
+  <si>
+    <t>Age-stratum-specific hospitalization (proportion of all (asymptomatic + symptomatic) infections that lead to hospitalisation) (%)</t>
+  </si>
+  <si>
+    <t>Relative percentage of regular daily contacts when hospitalised:</t>
+  </si>
+  <si>
+    <t>Self-isolation if Symptomatic</t>
+  </si>
+  <si>
+    <t>Template v12B</t>
+  </si>
+  <si>
+    <t>v12B changes:</t>
+  </si>
+  <si>
+    <t>Date range of simulation / Start:</t>
+  </si>
+  <si>
+    <t>Date range of simulation / End:</t>
+  </si>
+  <si>
+    <t>Probability of infection given contact:</t>
+  </si>
+  <si>
+    <t>Percentage of all asymptomatic infections that are reported:</t>
+  </si>
+  <si>
+    <t>Percentage of all symptomatic infections that are reported:</t>
+  </si>
+  <si>
+    <t>Percentage of all infections requiring hospitalisation that are actually admitted to hospital:</t>
+  </si>
+  <si>
+    <t>Added sheet "Parameters".</t>
+  </si>
+  <si>
+    <t>New parameters in v12 compared to v11 are hightlighted.</t>
+  </si>
+  <si>
+    <t>date_range_simul</t>
+  </si>
+  <si>
+    <t>date_range_simul_start</t>
+  </si>
+  <si>
+    <t>date_range_simul_end</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>reportc</t>
+  </si>
+  <si>
+    <t>reporth</t>
   </si>
   <si>
     <t>ihr_scaling</t>
   </si>
   <si>
-    <t>Screening/Overdispersion:</t>
-  </si>
-  <si>
-    <t>Screening/Contacts:</t>
-  </si>
-  <si>
-    <t>contacts</t>
-  </si>
-  <si>
-    <t>screen_overdispersion</t>
-  </si>
-  <si>
-    <t>screen_contacts</t>
-  </si>
-  <si>
-    <t>Days to implement maximum quarantine coverage:</t>
-  </si>
-  <si>
-    <t>quarantine_effort</t>
-  </si>
-  <si>
-    <t>Duration of hospitalised infection:</t>
-  </si>
-  <si>
-    <t>Duration of denied hospitalisation infection:</t>
-  </si>
-  <si>
-    <t>Duration of ICU infection:</t>
-  </si>
-  <si>
-    <t>Duration of denied ICU infection:</t>
-  </si>
-  <si>
-    <t>Duration of ventilated infection:</t>
-  </si>
-  <si>
-    <t>Duration of denied ventilation infection:</t>
-  </si>
-  <si>
-    <t>Note that new parameters in v12 compared to v11 are hightlighted.</t>
-  </si>
-  <si>
-    <t>Age-based relative fatality rate in well-resourced scenario (%)</t>
-  </si>
-  <si>
-    <t>Age-stratum-specific hospitalization (proportion of all (asymptomatic + symptomatic) infections that lead to hospitalisation) (%)</t>
-  </si>
-  <si>
-    <t>Relative percentage of regular daily contacts when hospitalised:</t>
-  </si>
-  <si>
-    <t>Self-isolation if Symptomatic</t>
+    <t>Scaling factor for infection hospitalisation rate: (NOT USED IN CURRENT VERSION)</t>
+  </si>
+  <si>
+    <t>Added mention (NOT USED IN CURRENT VERSION) to "Scaling factor for infection hospitalisation rate:" in Hospitalisation Parameters.</t>
   </si>
 </sst>
 </file>
@@ -2383,14 +2550,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2518,7 +2685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2575,6 +2742,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2890,20 +3063,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>210</v>
+      <c r="A1" s="28" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2926,9 +3099,57 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>226</v>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEFC6-D2C7-B343-A51D-3BA4E81D468A}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2944,7 +3165,7 @@
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4096,10 +4317,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4685,6 +4906,176 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEBEAC8-C0D6-3149-B965-10185C366694}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="37">
+        <v>43862</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="37">
+        <v>44075</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B93D921B-ACCD-B540-B62C-AE19092FA296}">
+      <formula1>0</formula1>
+      <formula2>0.2</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{25C6410D-5F17-2B45-9B47-570BD4117291}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{2B543E6D-BE7D-744F-84D2-DB111310B6BA}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{57FC95D5-98D8-714B-ACBA-F89D3090C305}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{439241F6-0612-BB4B-B5E3-5B6C55F0B4B9}">
+      <formula1>1</formula1>
+      <formula2>73051</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF179CC-EA38-1749-8906-36FC7049943A}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -4692,7 +5083,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4769,7 +5160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C67C35-2310-B341-9292-D007A3DFBE5D}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -4777,7 +5168,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4989,7 +5380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A51F038-D814-D045-99D6-939E07D55DA9}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -4997,7 +5388,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5079,7 +5470,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -5094,9 +5485,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>211</v>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>245</v>
       </c>
       <c r="B6" s="28">
         <v>1</v>
@@ -5106,7 +5497,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -5213,7 +5604,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -5230,7 +5621,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -5247,7 +5638,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -5264,7 +5655,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -5281,7 +5672,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -5298,7 +5689,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -5314,7 +5705,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B13:B18" xr:uid="{6C0631D2-5E94-0E44-AEDA-62F22487E25D}">
       <formula1>1</formula1>
       <formula2>30</formula2>
@@ -5325,13 +5716,9 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="B3:B4" xr:uid="{B281495F-DB35-47BB-9D76-CFF630A4B4E7}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B5 B7 B8:B12" xr:uid="{5D60B908-FEDB-4FEF-A945-3CA55E06C223}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B7:B12 B5" xr:uid="{5D60B908-FEDB-4FEF-A945-3CA55E06C223}">
       <formula1>0</formula1>
       <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{F0144E0F-4F43-4FA9-AFD5-45BD3B303306}">
-      <formula1>1</formula1>
-      <formula2>4</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5339,15 +5726,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173C6647-D12A-2647-B02F-0C6C0D519608}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5576,7 +5963,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="27" t="b">
@@ -5749,7 +6136,7 @@
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
       <c r="B21" s="31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -5761,13 +6148,13 @@
         <v>49</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
       <c r="B22" s="33" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5775,13 +6162,13 @@
         <v>4</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>49</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -6459,7 +6846,7 @@
     <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
       <c r="B58" s="35" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C58" s="29"/>
       <c r="D58" s="29"/>
@@ -6473,7 +6860,7 @@
         <v>49</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -6647,37 +7034,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEFC6-D2C7-B343-A51D-3BA4E81D468A}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update social contact via template
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6E9271-46FE-0B40-BCAA-49E86F518634}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76890B40-42FE-7E40-BFB6-88D9A64986B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="460" windowWidth="20700" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -382,12 +382,54 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-0 - 100%</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="1" shapeId="0" xr:uid="{CAFDEB5A-367C-214E-9860-6419D337CBE9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1, 2, 3 or 4.</t>
         </r>
       </text>
     </comment>
@@ -1726,7 +1768,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="404">
   <si>
     <t>date</t>
   </si>
@@ -2409,12 +2451,6 @@
     <t>Self-isolation if Symptomatic</t>
   </si>
   <si>
-    <t>Template v12B</t>
-  </si>
-  <si>
-    <t>v12B changes:</t>
-  </si>
-  <si>
     <t>Date range of simulation / Start:</t>
   </si>
   <si>
@@ -2436,9 +2472,6 @@
     <t>Added sheet "Parameters".</t>
   </si>
   <si>
-    <t>New parameters in v12 compared to v11 are hightlighted.</t>
-  </si>
-  <si>
     <t>date_range_simul</t>
   </si>
   <si>
@@ -2467,6 +2500,486 @@
   </si>
   <si>
     <t>Added mention (NOT USED IN CURRENT VERSION) to "Scaling factor for infection hospitalisation rate:" in Hospitalisation Parameters.</t>
+  </si>
+  <si>
+    <t>Social Contacts</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia (Plurinational State of</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hong Kong SAR, China</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran (Islamic Republic of)</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republi</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Republic of Korea</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sao Tome and Principe </t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>TFYR of Macedonia</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom of Great Britain</t>
+  </si>
+  <si>
+    <t>United Republic of Tanzania</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela (Bolivarian Republic </t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Social Contacts Data:</t>
+  </si>
+  <si>
+    <t>Value_Country</t>
+  </si>
+  <si>
+    <t>picker</t>
+  </si>
+  <si>
+    <t>country_contact</t>
+  </si>
+  <si>
+    <t>Added Social Contacts Data parameter in sheet "Country Area Parameters".</t>
+  </si>
+  <si>
+    <t>Template v12-B</t>
+  </si>
+  <si>
+    <t>v12-B changes:</t>
   </si>
 </sst>
 </file>
@@ -2477,7 +2990,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2556,6 +3069,19 @@
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -2685,7 +3211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2742,11 +3268,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3063,10 +3590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3076,7 +3603,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>227</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3101,22 +3628,22 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>228</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3126,10 +3653,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEFC6-D2C7-B343-A51D-3BA4E81D468A}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3137,19 +3664,778 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C83" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C84" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C85" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C86" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C87" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C88" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C89" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C90" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C91" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C92" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C93" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C94" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C95" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C96" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C97" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C98" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C99" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C100" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C101" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C102" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C103" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C104" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C105" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C106" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C107" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C108" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C109" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C110" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C111" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C112" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C113" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C114" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C115" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C116" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C117" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C118" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C119" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C120" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C121" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C122" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C123" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C124" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C125" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C126" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C127" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C128" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C129" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C130" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C131" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C132" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C133" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C134" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C135" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C136" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C137" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C138" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C139" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C140" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C141" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C142" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C143" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C144" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C145" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C146" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C147" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C148" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C149" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C150" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C151" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C152" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C153" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -4302,7 +5588,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4912,8 +6198,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4948,7 +6234,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B2" s="37">
         <v>43862</v>
@@ -4956,15 +6242,15 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B3" s="37">
         <v>44075</v>
@@ -4972,15 +6258,15 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4">
@@ -4991,12 +6277,12 @@
         <v>49</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5">
@@ -5009,12 +6295,12 @@
         <v>49</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6">
@@ -5027,12 +6313,12 @@
         <v>49</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7">
@@ -5045,7 +6331,7 @@
         <v>49</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5080,83 +6366,117 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>386</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="3"/>
+      <c r="C3">
         <v>2.8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{A2B6A4A1-21F7-44BD-A536-4E6AFE445B59}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{A2B6A4A1-21F7-44BD-A536-4E6AFE445B59}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{931327C6-46CF-4FD3-BA8F-07E73A7543F5}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{931327C6-46CF-4FD3-BA8F-07E73A7543F5}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7715037C-2AB5-744F-90C5-E7A36E8197AB}">
+          <x14:formula1>
+            <xm:f>HIDDEN!$C$2:$C$153</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5388,7 +6708,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5486,10 +6806,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="B6" s="28">
+      <c r="A6" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="3"/>
@@ -5497,7 +6817,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -5705,7 +7025,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B13:B18" xr:uid="{6C0631D2-5E94-0E44-AEDA-62F22487E25D}">
       <formula1>1</formula1>
       <formula2>30</formula2>
@@ -5719,6 +7039,10 @@
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B7:B12 B5" xr:uid="{5D60B908-FEDB-4FEF-A945-3CA55E06C223}">
       <formula1>0</formula1>
       <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{B4ABC229-799B-514E-B7F5-8FD96E5E9CBE}">
+      <formula1>1</formula1>
+      <formula2>4</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added horizontal line at Rt = 1
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76890B40-42FE-7E40-BFB6-88D9A64986B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614404C0-F04E-E64A-84D5-B560865FCF1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2979,7 +2979,7 @@
     <t>Template v12-B</t>
   </si>
   <si>
-    <t>v12-B changes:</t>
+    <t>Changes in v12-B:</t>
   </si>
 </sst>
 </file>
@@ -3593,7 +3593,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6708,7 +6708,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Dropdown TRUE/FALSE for interventions
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614404C0-F04E-E64A-84D5-B560865FCF1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0F1C3F-A275-DA4F-A874-54EA28152C96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -900,7 +900,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -909,12 +909,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 - 5</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 - 5</t>
         </r>
       </text>
     </comment>
@@ -924,7 +933,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -933,12 +942,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 - 10</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 - 10</t>
         </r>
       </text>
     </comment>
@@ -3211,7 +3229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3251,19 +3269,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -3274,6 +3279,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3592,8 +3612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3642,7 +3662,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="33" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3655,7 +3675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEFC6-D2C7-B343-A51D-3BA4E81D468A}">
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
@@ -6198,7 +6218,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -6236,7 +6256,7 @@
       <c r="A2" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="30">
         <v>43862</v>
       </c>
       <c r="C2" s="3"/>
@@ -6252,7 +6272,7 @@
       <c r="A3" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="30">
         <v>44075</v>
       </c>
       <c r="C3" s="3"/>
@@ -6406,7 +6426,7 @@
       <c r="A2" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="34" t="s">
         <v>386</v>
       </c>
       <c r="C2" s="6"/>
@@ -6806,7 +6826,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="35" t="s">
         <v>242</v>
       </c>
       <c r="B6">
@@ -7058,7 +7078,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7122,7 +7142,7 @@
         <v>200</v>
       </c>
       <c r="B3" s="19"/>
-      <c r="C3" s="36" t="b">
+      <c r="C3" s="29" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="3"/>
@@ -7141,7 +7161,7 @@
         <v>119</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="37">
+      <c r="D4" s="30">
         <v>43913</v>
       </c>
       <c r="E4" s="3"/>
@@ -7178,7 +7198,7 @@
         <v>201</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="36" t="b">
+      <c r="C6" s="29" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="3"/>
@@ -7197,7 +7217,7 @@
         <v>119</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="37">
+      <c r="D7" s="30">
         <v>43913</v>
       </c>
       <c r="E7" s="3"/>
@@ -7234,7 +7254,7 @@
         <v>202</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="C9" s="36" t="b">
+      <c r="C9" s="29" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="3"/>
@@ -7253,7 +7273,7 @@
         <v>119</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="37">
+      <c r="D10" s="30">
         <v>43913</v>
       </c>
       <c r="E10" s="3"/>
@@ -7272,7 +7292,7 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="38">
+      <c r="E11" s="31">
         <v>3</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -7309,7 +7329,7 @@
         <v>119</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="37">
+      <c r="D13" s="30">
         <v>43902</v>
       </c>
       <c r="E13" s="3"/>
@@ -7405,7 +7425,7 @@
         <v>157</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="37">
+      <c r="D18" s="30">
         <v>44196</v>
       </c>
       <c r="E18" s="3"/>
@@ -7444,7 +7464,7 @@
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="39">
+      <c r="E20" s="32">
         <v>32</v>
       </c>
       <c r="F20" s="12" t="s">
@@ -7458,13 +7478,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="42">
         <v>4</v>
       </c>
       <c r="F21" s="12"/>
@@ -7476,13 +7496,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34">
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="43">
         <v>4</v>
       </c>
       <c r="F22" s="14" t="s">
@@ -7519,7 +7539,7 @@
         <v>119</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="37">
+      <c r="D24" s="30">
         <v>43906</v>
       </c>
       <c r="E24" s="3"/>
@@ -7578,7 +7598,7 @@
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
-      <c r="E27" s="38">
+      <c r="E27" s="31">
         <v>100</v>
       </c>
       <c r="F27" s="14" t="s">
@@ -7615,7 +7635,7 @@
         <v>119</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="37">
+      <c r="D29" s="30">
         <v>43894</v>
       </c>
       <c r="E29" s="3"/>
@@ -7654,7 +7674,7 @@
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="38">
+      <c r="E31" s="31">
         <v>5</v>
       </c>
       <c r="F31" s="14" t="s">
@@ -7691,7 +7711,7 @@
         <v>119</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="37">
+      <c r="D33" s="30">
         <v>43909</v>
       </c>
       <c r="E33" s="3"/>
@@ -7770,7 +7790,7 @@
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
-      <c r="E37" s="38">
+      <c r="E37" s="31">
         <v>10</v>
       </c>
       <c r="F37" s="14" t="s">
@@ -7807,7 +7827,7 @@
         <v>119</v>
       </c>
       <c r="C39" s="3"/>
-      <c r="D39" s="37">
+      <c r="D39" s="30">
         <v>43910</v>
       </c>
       <c r="E39" s="3"/>
@@ -7866,7 +7886,7 @@
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
-      <c r="E42" s="38">
+      <c r="E42" s="31">
         <v>20</v>
       </c>
       <c r="F42" s="14" t="s">
@@ -7903,7 +7923,7 @@
         <v>119</v>
       </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="37">
+      <c r="D44" s="30">
         <v>43911</v>
       </c>
       <c r="E44" s="3"/>
@@ -7982,7 +8002,7 @@
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="38">
+      <c r="E48" s="31">
         <v>70</v>
       </c>
       <c r="F48" s="14" t="s">
@@ -8019,7 +8039,7 @@
         <v>119</v>
       </c>
       <c r="C50" s="3"/>
-      <c r="D50" s="37">
+      <c r="D50" s="30">
         <v>44196</v>
       </c>
       <c r="E50" s="3"/>
@@ -8058,7 +8078,7 @@
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
-      <c r="E52" s="38">
+      <c r="E52" s="31">
         <v>50</v>
       </c>
       <c r="F52" s="14" t="s">
@@ -8095,7 +8115,7 @@
         <v>119</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="37">
+      <c r="D54" s="30">
         <v>43908</v>
       </c>
       <c r="E54" s="3"/>
@@ -8169,12 +8189,12 @@
     </row>
     <row r="58" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29">
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="42">
         <v>2</v>
       </c>
       <c r="F58" s="12" t="s">
@@ -8214,7 +8234,7 @@
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
-      <c r="E60" s="38">
+      <c r="E60" s="31">
         <v>100</v>
       </c>
       <c r="F60" s="14" t="s">
@@ -8251,7 +8271,7 @@
         <v>119</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="37">
+      <c r="D62" s="30">
         <v>44348</v>
       </c>
       <c r="E62" s="3"/>
@@ -8310,7 +8330,7 @@
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
-      <c r="E65" s="38">
+      <c r="E65" s="31">
         <v>0</v>
       </c>
       <c r="F65" s="14" t="s">
@@ -8357,5 +8377,17 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D9C273A-8170-CB49-8167-9B2AD22225CB}">
+          <x14:formula1>
+            <xm:f>HIDDEN!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3 C6 C9 C12 C17 C23 C28 C32 C38 C43 C49 C53 C61</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allow smaller time range
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D20FFC-FD1F-9E4F-A05F-B0D4534BF210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FBE169-5172-F848-8276-861B6F919ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3666,7 +3666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -4524,7 +4524,7 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -7131,7 +7131,7 @@
   </sheetPr>
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
set reporth default value to 100
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FBE169-5172-F848-8276-861B6F919ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3049F1BC-BE35-AF44-BDBF-804687064AC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="27980" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3666,7 +3666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -6272,8 +6272,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>55</v>
@@ -6409,7 +6409,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B93D921B-ACCD-B540-B62C-AE19092FA296}">
       <formula1>0</formula1>
       <formula2>0.2</formula2>

</xml_diff>

<commit_message>
Move interventions parameters to pushbar
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27787D2D-CBDC-5E49-9559-08062512871F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77859F27-2AED-5742-847F-6EFF450017BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="648" firstSheet="1" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="14920" yWindow="-21140" windowWidth="17640" windowHeight="21140" tabRatio="648" firstSheet="6" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2975,8 +2975,8 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6910,8 +6910,8 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7409,7 +7409,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H27" xr:uid="{E454A1AF-76A4-7D40-98C2-916796BE8673}"/>
-  <dataValidations count="6">
+  <dataValidations disablePrompts="1" count="6">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6" xr:uid="{E2FA9153-BF97-F44D-8444-660C47A52190}">
       <formula1>1</formula1>
       <formula2>10</formula2>
@@ -7439,7 +7439,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D9C273A-8170-CB49-8167-9B2AD22225CB}">
           <x14:formula1>
             <xm:f>HIDDEN!$A$2:$A$3</xm:f>

</xml_diff>

<commit_message>
extended to 30 interventions
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3345A7-C933-674E-9CF8-DFC1790A96B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8525FDCD-80F2-2948-96CC-980ED1DADB3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="-21140" windowWidth="16220" windowHeight="21140" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="-4580" yWindow="-21140" windowWidth="38280" windowHeight="21140" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1201,7 +1201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="352">
   <si>
     <t>date</t>
   </si>
@@ -2984,10 +2984,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3022,13 +3022,13 @@
         <v>111</v>
       </c>
       <c r="B2" s="7">
-        <v>43466</v>
+        <v>43876</v>
       </c>
       <c r="C2" s="7">
-        <v>43525</v>
+        <v>43936</v>
       </c>
       <c r="D2" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>345</v>
@@ -3036,16 +3036,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B3" s="7">
-        <v>43526</v>
+        <v>43937</v>
       </c>
       <c r="C3" s="7">
-        <v>43831</v>
+        <v>44196</v>
       </c>
       <c r="D3" s="1">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>345</v>
@@ -3053,16 +3053,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B4" s="7">
-        <v>44013</v>
+        <v>43866</v>
       </c>
       <c r="C4" s="7">
-        <v>44044</v>
+        <v>43890</v>
       </c>
       <c r="D4" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>345</v>
@@ -3070,67 +3070,67 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="B5" s="7">
-        <v>43556</v>
+        <v>43891</v>
       </c>
       <c r="C5" s="7">
-        <v>43586</v>
+        <v>44012</v>
       </c>
       <c r="D5" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="B6" s="7">
-        <v>43466</v>
+        <v>43876</v>
       </c>
       <c r="C6" s="7">
-        <v>43525</v>
+        <v>43921</v>
       </c>
       <c r="D6" s="1">
         <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="B7" s="7">
-        <v>43101</v>
+        <v>43922</v>
       </c>
       <c r="C7" s="7">
-        <v>43622</v>
+        <v>44012</v>
       </c>
       <c r="D7" s="1">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="B8" s="7">
-        <v>43511</v>
+        <v>43961</v>
       </c>
       <c r="C8" s="7">
-        <v>43586</v>
+        <v>43982</v>
       </c>
       <c r="D8" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>351</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="B9" s="7">
-        <v>43587</v>
+        <v>43983</v>
       </c>
       <c r="C9" s="7">
-        <v>43617</v>
+        <v>44012</v>
       </c>
       <c r="D9" s="1">
         <v>100</v>
@@ -3154,18 +3154,38 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="7">
+        <v>44013</v>
+      </c>
+      <c r="C10" s="7">
+        <v>44074</v>
+      </c>
+      <c r="D10" s="1">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="7">
+        <v>44075</v>
+      </c>
+      <c r="C11" s="7">
+        <v>44104</v>
+      </c>
+      <c r="D11" s="1">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -3433,9 +3453,16 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D49" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3448,13 +3475,13 @@
           <x14:formula1>
             <xm:f>HIDDEN!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E49</xm:sqref>
+          <xm:sqref>E2:E50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47936E1B-CEB7-1140-B286-248EE55FD596}">
           <x14:formula1>
             <xm:f>HIDDEN!$E$2:$E$14</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A49</xm:sqref>
+          <xm:sqref>A2:A50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6070,7 +6097,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6123,7 +6150,7 @@
         <v>167</v>
       </c>
       <c r="B3" s="7">
-        <v>44075</v>
+        <v>44196</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>169</v>

</xml_diff>

<commit_message>
rewrite timevis for baseline
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8525FDCD-80F2-2948-96CC-980ED1DADB3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4D7B37-A611-9B4E-9441-B364ACB2156D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4580" yWindow="-21140" windowWidth="38280" windowHeight="21140" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="13260" yWindow="-21140" windowWidth="20440" windowHeight="21140" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -2986,7 +2986,7 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -6096,8 +6096,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed 3 parameters duration denied
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A91D14-9965-1C4D-B776-549D5728AC91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3615C25E-9419-3146-BBD4-1218C15906E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="-21140" windowWidth="20440" windowHeight="21140" tabRatio="648" firstSheet="3" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="17540" tabRatio="648" activeTab="7" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Hospitalisation Param" sheetId="9" r:id="rId8"/>
     <sheet name="Interventions Param" sheetId="11" r:id="rId9"/>
     <sheet name="Interventions" sheetId="14" r:id="rId10"/>
-    <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId11"/>
+    <sheet name="HIDDEN" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$27</definedName>
@@ -476,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="1" shapeId="0" xr:uid="{96AD9494-0E73-EB4D-B4E7-5944E1089063}">
+    <comment ref="B14" authorId="1" shapeId="0" xr:uid="{6AF90CD2-69CC-AA4B-A769-14DADD96C490}">
       <text>
         <r>
           <rPr>
@@ -509,106 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="1" shapeId="0" xr:uid="{6AF90CD2-69CC-AA4B-A769-14DADD96C490}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="1" shapeId="0" xr:uid="{15100A51-88F1-2D4A-BE13-B9EA8C6490CE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="1" shapeId="0" xr:uid="{5813D783-EA21-DD45-B6C5-56D42BCEDA80}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>1 to 30 days</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="1" shapeId="0" xr:uid="{0F7FC5C6-6ECF-DF4D-84D6-9F029454BE66}">
+    <comment ref="B15" authorId="1" shapeId="0" xr:uid="{5813D783-EA21-DD45-B6C5-56D42BCEDA80}">
       <text>
         <r>
           <rPr>
@@ -1201,7 +1102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="345">
   <si>
     <t>date</t>
   </si>
@@ -1365,9 +1266,6 @@
     <t>beds_available</t>
   </si>
   <si>
-    <t>Maximum number of hospital beds</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -1470,33 +1368,15 @@
     <t>nus</t>
   </si>
   <si>
-    <t>nusc</t>
-  </si>
-  <si>
-    <t>nu_icuc</t>
-  </si>
-  <si>
     <t>nu_vent</t>
   </si>
   <si>
-    <t>nu_ventc</t>
-  </si>
-  <si>
     <t>nu_icu</t>
   </si>
   <si>
     <t>beds</t>
   </si>
   <si>
-    <t>ventilators</t>
-  </si>
-  <si>
-    <t>Maximum number of ICU beds</t>
-  </si>
-  <si>
-    <t>Maximum number of ventilators</t>
-  </si>
-  <si>
     <t>Probability of dying when hospitalised:</t>
   </si>
   <si>
@@ -1674,19 +1554,10 @@
     <t>Duration of hospitalised infection:</t>
   </si>
   <si>
-    <t>Duration of denied hospitalisation infection:</t>
-  </si>
-  <si>
     <t>Duration of ICU infection:</t>
   </si>
   <si>
-    <t>Duration of denied ICU infection:</t>
-  </si>
-  <si>
     <t>Duration of ventilated infection:</t>
-  </si>
-  <si>
-    <t>Duration of denied ventilation infection:</t>
   </si>
   <si>
     <t>Age-based relative fatality rate in well-resourced scenario (%)</t>
@@ -2303,6 +2174,61 @@
   </si>
   <si>
     <t>Future Scenario</t>
+  </si>
+  <si>
+    <t>Maximum number of hospital surge beds</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum number of ICU beds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>without</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ventilators</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum number of ICU beds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ventilators</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2535,7 +2461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2566,9 +2492,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2622,6 +2545,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2941,7 +2868,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2951,27 +2878,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2986,8 +2913,8 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3002,24 +2929,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" s="7">
         <v>43876</v>
@@ -3031,12 +2958,12 @@
         <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B3" s="7">
         <v>43937</v>
@@ -3048,12 +2975,12 @@
         <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7">
         <v>43866</v>
@@ -3065,12 +2992,12 @@
         <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B5" s="7">
         <v>43891</v>
@@ -3082,12 +3009,12 @@
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -3099,12 +3026,12 @@
         <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B7" s="7">
         <v>43922</v>
@@ -3116,12 +3043,12 @@
         <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B8" s="7">
         <v>43961</v>
@@ -3133,12 +3060,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B9" s="7">
         <v>43983</v>
@@ -3150,12 +3077,12 @@
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B10" s="7">
         <v>44013</v>
@@ -3167,12 +3094,12 @@
         <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B11" s="7">
         <v>44075</v>
@@ -3184,7 +3111,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3494,7 +3421,7 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3506,16 +3433,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3523,13 +3450,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3537,796 +3464,796 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73" s="2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" s="2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="2" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" s="2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="2" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" s="2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C114" s="2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C116" s="2" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C118" s="2" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C119" s="2" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C120" s="2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="2" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C122" s="2" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C124" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="2" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C126" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C127" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="2" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="2" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="2" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="2" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="2" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="2" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C148" s="2" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C149" s="2" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C150" s="2" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C151" s="2" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C152" s="2" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C153" s="2" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -4356,10 +4283,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5483,7 +5410,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5499,10 +5426,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5773,13 +5700,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6116,13 +6043,13 @@
         <v>23</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>44</v>
@@ -6133,35 +6060,35 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B2" s="7">
         <v>43862</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B3" s="7">
         <v>44196</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C4" s="1">
         <v>4.9000000000000002E-2</v>
@@ -6170,58 +6097,58 @@
         <v>49</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="C5" s="1">
         <v>2.5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C7" s="1">
         <v>50</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -6278,13 +6205,13 @@
         <v>23</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>44</v>
@@ -6295,29 +6222,29 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="14" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>2.8</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>49</v>
@@ -6328,13 +6255,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>46</v>
@@ -6399,7 +6326,7 @@
         <v>47</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>44</v>
@@ -6409,14 +6336,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>59</v>
+      <c r="A2" s="43" t="s">
+        <v>58</v>
       </c>
       <c r="B2" s="12">
         <v>10</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>49</v>
@@ -6426,14 +6353,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
-        <v>58</v>
+      <c r="A3" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="B3" s="12">
         <v>3.5</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>49</v>
@@ -6443,120 +6370,120 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
-        <v>63</v>
+      <c r="A4" s="43" t="s">
+        <v>62</v>
       </c>
       <c r="B4" s="12">
         <v>4.5</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
-        <v>65</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="14" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="43" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
-        <v>68</v>
-      </c>
       <c r="B6" s="12">
         <v>0</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
-        <v>70</v>
       </c>
       <c r="B7" s="12">
         <v>150</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
-        <v>73</v>
+      <c r="A8" s="43" t="s">
+        <v>72</v>
       </c>
       <c r="B8" s="12">
         <v>55</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
-        <v>75</v>
       </c>
       <c r="B9" s="12">
         <v>50</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="43" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>77</v>
       </c>
       <c r="B10" s="12">
         <v>75</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6596,16 +6523,16 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -6620,7 +6547,7 @@
         <v>47</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>44</v>
@@ -6631,13 +6558,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="1">
+        <v>342</v>
+      </c>
+      <c r="B2" s="44">
         <v>160000</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>46</v>
@@ -6648,58 +6575,58 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="1">
+        <v>343</v>
+      </c>
+      <c r="B3" s="44">
         <v>8000</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="1">
+        <v>344</v>
+      </c>
+      <c r="B4" s="44">
         <v>8000</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>177</v>
+      <c r="A6" s="45" t="s">
+        <v>167</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -6708,137 +6635,137 @@
         <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1">
         <v>35</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1">
         <v>45</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B9" s="1">
         <v>55</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1">
         <v>80</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B11" s="1">
         <v>80</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1">
         <v>95</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>49</v>
@@ -6849,78 +6776,23 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B13:B18" xr:uid="{6C0631D2-5E94-0E44-AEDA-62F22487E25D}">
-      <formula1>1</formula1>
-      <formula2>30</formula2>
-    </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{1D15A7CB-72A1-4F2B-8C53-02E77DE5D83B}">
       <formula1>1</formula1>
     </dataValidation>
@@ -6934,6 +6806,10 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{B4ABC229-799B-514E-B7F5-8FD96E5E9CBE}">
       <formula1>1</formula1>
       <formula2>4</formula2>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{6C0631D2-5E94-0E44-AEDA-62F22487E25D}">
+      <formula1>1</formula1>
+      <formula2>30</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6965,16 +6841,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>44</v>
@@ -6984,397 +6860,397 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="39" t="s">
-        <v>121</v>
+      <c r="A3" s="18"/>
+      <c r="B3" s="38" t="s">
+        <v>114</v>
       </c>
       <c r="C3" s="12">
         <v>50</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>118</v>
+      <c r="F3" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="A4" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="41" t="s">
-        <v>349</v>
-      </c>
-      <c r="C5" s="33">
+      <c r="A5" s="21"/>
+      <c r="B5" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="C5" s="32">
         <v>4</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>152</v>
+      <c r="F5" s="20" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="42" t="s">
-        <v>350</v>
-      </c>
-      <c r="C6" s="34">
+      <c r="A6" s="22"/>
+      <c r="B6" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="33">
         <v>4</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="D6" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>153</v>
+      <c r="F6" s="24" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="A7" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="34">
         <v>100</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="24" t="s">
+      <c r="D8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>119</v>
+      <c r="F8" s="24" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="A9" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="39" t="s">
-        <v>122</v>
+      <c r="A10" s="18"/>
+      <c r="B10" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="C10" s="12">
         <v>85</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="D10" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>120</v>
+      <c r="F10" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="34">
         <v>10</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>124</v>
+      <c r="F11" s="24" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
+      <c r="A12" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="39" t="s">
-        <v>122</v>
+      <c r="A13" s="18"/>
+      <c r="B13" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="C13" s="12">
         <v>85</v>
       </c>
-      <c r="D13" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="20" t="s">
+      <c r="D13" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>126</v>
+      <c r="F13" s="20" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="34">
         <v>20</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="24" t="s">
+      <c r="D14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>127</v>
+      <c r="F14" s="24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>338</v>
-      </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="A15" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="39" t="s">
-        <v>122</v>
+      <c r="A16" s="18"/>
+      <c r="B16" s="38" t="s">
+        <v>115</v>
       </c>
       <c r="C16" s="12">
         <v>95</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="20" t="s">
+      <c r="D16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="C17" s="34">
+        <v>70</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="34">
+        <v>50</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="38" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="43" t="s">
-        <v>339</v>
-      </c>
-      <c r="C17" s="35">
-        <v>70</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="35">
-        <v>50</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
-    </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="39" t="s">
-        <v>135</v>
       </c>
       <c r="C21" s="12">
         <v>14</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="20" t="s">
+      <c r="D21" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="21" t="s">
-        <v>132</v>
+      <c r="F21" s="20" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="33">
+      <c r="A22" s="18"/>
+      <c r="B22" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="32">
         <v>2</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="21" t="s">
-        <v>155</v>
+      <c r="F22" s="20" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="39" t="s">
-        <v>136</v>
+      <c r="A23" s="18"/>
+      <c r="B23" s="38" t="s">
+        <v>129</v>
       </c>
       <c r="C23" s="12">
         <v>20</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="20" t="s">
+      <c r="D23" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="21" t="s">
-        <v>133</v>
+      <c r="F23" s="20" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="35">
+      <c r="A24" s="25"/>
+      <c r="B24" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="34">
         <v>100</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="24" t="s">
+      <c r="D24" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>134</v>
+      <c r="F24" s="24" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="A25" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
-      <c r="B26" s="39" t="s">
-        <v>139</v>
+      <c r="A26" s="18"/>
+      <c r="B26" s="38" t="s">
+        <v>132</v>
       </c>
       <c r="C26" s="12">
         <v>4</v>
       </c>
-      <c r="D26" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>140</v>
+      <c r="F26" s="20" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="35">
-        <v>0</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="24" t="s">
+      <c r="A27" s="25"/>
+      <c r="B27" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="34">
+        <v>0</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="25" t="s">
-        <v>141</v>
+      <c r="F27" s="24" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start to bridge with v13.3
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21E05CC-25B3-6941-9C65-474E14F06F53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C072E98-A851-0E4B-BC8D-3E7276C53CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="17540" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -637,7 +637,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2A3F5E2F-D961-4C00-8CF7-801F8593082C}">
+    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{B4AB7C2D-B141-D140-A03F-72A8E66AFC89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 to 5 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{DC6047C5-CC94-4D39-B8F5-D8E1BC59DC13}">
       <text>
         <r>
           <rPr>
@@ -666,11 +699,209 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 - 10</t>
+          <t>0 - 100%</t>
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="1" shapeId="0" xr:uid="{B4AB7C2D-B141-D140-A03F-72A8E66AFC89}">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{DA868374-A6F9-41A4-8E01-641686A7BCD8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{33ECC315-8C1C-412A-93E2-AC949FE3FD96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{C52EBBE4-D1FF-4590-95C6-438370A19E03}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{59D86E4D-23E3-4A93-9A15-CFE70D521E51}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{05F414A2-8255-46E3-9C62-928679F11C53}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{728217A9-5FAF-4A64-8758-A31064D2AA76}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0 - 100%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="1" shapeId="0" xr:uid="{46D2EC60-D9BF-5B4B-8A58-5ABB2239D72B}">
       <text>
         <r>
           <rPr>
@@ -699,11 +930,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 to 5 days</t>
+          <t>0 to 100 y.o.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{DC6047C5-CC94-4D39-B8F5-D8E1BC59DC13}">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{BCC3B568-B0F7-4053-884F-6FAF392D69F9}">
       <text>
         <r>
           <rPr>
@@ -736,21 +967,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{DA868374-A6F9-41A4-8E01-641686A7BCD8}">
+    <comment ref="C28" authorId="1" shapeId="0" xr:uid="{7ABCA5E8-93BC-7C4B-A47B-29E3D179384F}">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Olivier Celhay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -760,281 +991,17 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 to 52 weeks
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{33ECC315-8C1C-412A-93E2-AC949FE3FD96}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{C52EBBE4-D1FF-4590-95C6-438370A19E03}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{59D86E4D-23E3-4A93-9A15-CFE70D521E51}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{05F414A2-8255-46E3-9C62-928679F11C53}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{728217A9-5FAF-4A64-8758-A31064D2AA76}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C25" authorId="1" shapeId="0" xr:uid="{46D2EC60-D9BF-5B4B-8A58-5ABB2239D72B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 to 100 y.o.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{BCC3B568-B0F7-4053-884F-6FAF392D69F9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>0 - 100%</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C29" authorId="1" shapeId="0" xr:uid="{7ABCA5E8-93BC-7C4B-A47B-29E3D179384F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Olivier Celhay:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">1 to 52 weeks
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{936A1F9D-AF0C-4AEA-9081-4A1A7E608056}">
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{936A1F9D-AF0C-4AEA-9081-4A1A7E608056}">
       <text>
         <r>
           <rPr>
@@ -1072,7 +1039,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="343">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1485,13 +1452,7 @@
     <t>Deaths per person per day</t>
   </si>
   <si>
-    <t>contacts</t>
-  </si>
-  <si>
     <t>screen_overdispersion</t>
-  </si>
-  <si>
-    <t>screen_contacts</t>
   </si>
   <si>
     <t>Days to implement maximum quarantine coverage:</t>
@@ -2110,9 +2071,6 @@
     <t>Overdispersion:</t>
   </si>
   <si>
-    <t>Contacts:</t>
-  </si>
-  <si>
     <t>Maximum number of hospital surge beds</t>
   </si>
   <si>
@@ -2199,6 +2157,9 @@
   </si>
   <si>
     <t>hand_eff</t>
+  </si>
+  <si>
+    <t>Efficacy: (0-25%)</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2453,7 +2414,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2468,9 +2428,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2492,9 +2449,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2835,7 +2789,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2886,19 +2840,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>328</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2915,7 +2869,7 @@
         <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2932,7 +2886,7 @@
         <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2949,7 +2903,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,12 +2920,12 @@
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -2983,12 +2937,12 @@
         <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B7" s="7">
         <v>43876</v>
@@ -3000,12 +2954,12 @@
         <v>90</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B8" s="7">
         <v>43876</v>
@@ -3017,7 +2971,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3034,7 +2988,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3051,7 +3005,7 @@
         <v>90</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3068,7 +3022,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3085,12 +3039,12 @@
         <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="7">
         <v>43876</v>
@@ -3102,12 +3056,12 @@
         <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B14" s="7">
         <v>43876</v>
@@ -3119,12 +3073,12 @@
         <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B15" s="7">
         <v>43876</v>
@@ -3136,12 +3090,12 @@
         <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B16" s="7">
         <v>43876</v>
@@ -3153,7 +3107,7 @@
         <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3443,13 +3397,13 @@
         <v>131</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3457,13 +3411,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3471,26 +3425,26 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>101</v>
@@ -3498,7 +3452,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>102</v>
@@ -3506,7 +3460,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>103</v>
@@ -3514,7 +3468,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>104</v>
@@ -3522,23 +3476,23 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>127</v>
@@ -3546,712 +3500,712 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C114" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C116" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C118" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C119" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C120" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C122" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C124" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C126" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C127" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C148" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C149" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C150" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C151" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C152" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C153" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4278,7 +4232,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>133</v>
@@ -5419,13 +5373,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="170" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5693,7 +5647,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>134</v>
@@ -6056,35 +6010,35 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" s="7">
         <v>43862</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="7">
         <v>44196</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>152</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1">
         <v>4.9000000000000002E-2</v>
@@ -6093,12 +6047,12 @@
         <v>47</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C5" s="1">
         <v>2.5</v>
@@ -6110,12 +6064,12 @@
         <v>47</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -6127,12 +6081,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1">
         <v>50</v>
@@ -6144,7 +6098,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6201,7 +6155,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>45</v>
@@ -6218,18 +6172,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6332,7 +6286,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="12">
@@ -6349,7 +6303,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="12">
@@ -6366,7 +6320,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="40" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="12">
@@ -6383,7 +6337,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="12">
@@ -6398,7 +6352,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="40" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="12">
@@ -6415,7 +6369,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="40" t="s">
         <v>67</v>
       </c>
       <c r="B7" s="12">
@@ -6432,7 +6386,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="40" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="12">
@@ -6449,7 +6403,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="40" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="12">
@@ -6466,7 +6420,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="12">
@@ -6554,9 +6508,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="B2" s="44">
+        <v>328</v>
+      </c>
+      <c r="B2" s="41">
         <v>160000</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -6571,9 +6525,9 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="B3" s="44">
+        <v>329</v>
+      </c>
+      <c r="B3" s="41">
         <v>8000</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -6588,9 +6542,9 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="B4" s="44">
+        <v>330</v>
+      </c>
+      <c r="B4" s="41">
         <v>8000</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -6605,7 +6559,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -6621,8 +6575,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
-        <v>160</v>
+      <c r="A6" s="42" t="s">
+        <v>158</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -6631,7 +6585,7 @@
         <v>47</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -6738,7 +6692,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -6755,7 +6709,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -6772,7 +6726,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -6818,10 +6772,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6856,24 +6810,24 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="A2" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>110</v>
       </c>
       <c r="C3" s="12">
         <v>50</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="33" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="19" t="s">
@@ -6884,436 +6838,414 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30"/>
+      <c r="A4" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
-      <c r="B5" s="40" t="s">
-        <v>329</v>
-      </c>
-      <c r="C5" s="32">
+      <c r="B5" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="31">
         <v>4</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
-      <c r="B6" s="40" t="s">
-        <v>342</v>
-      </c>
-      <c r="C6" s="32">
+      <c r="B6" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" s="31">
         <v>80</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="33" t="s">
         <v>52</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="41" t="s">
-        <v>330</v>
-      </c>
-      <c r="C7" s="33">
-        <v>4</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="12">
+        <v>14</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>335</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="20" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="12">
-        <v>14</v>
-      </c>
-      <c r="D9" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="31">
+        <v>2</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>53</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
-      <c r="B10" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="32">
-        <v>2</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>53</v>
+      <c r="B10" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="12">
+        <v>20</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="12">
-        <v>20</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="32">
+        <v>100</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="34">
+      <c r="F11" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="32">
         <v>100</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="34">
-        <v>100</v>
-      </c>
-      <c r="D14" s="37" t="s">
+      <c r="F13" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" s="32">
+        <v>5</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-    </row>
-    <row r="16" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="38" t="s">
+      <c r="F15" s="23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C17" s="12">
         <v>85</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D17" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="24" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="12">
-        <v>85</v>
+      <c r="F17" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="32">
+        <v>10</v>
       </c>
       <c r="D18" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="34">
-        <v>10</v>
-      </c>
-      <c r="D19" s="37" t="s">
+      <c r="F18" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="12">
+        <v>85</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="12">
-        <v>85</v>
+      <c r="F20" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="32">
+        <v>20</v>
       </c>
       <c r="D21" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="34">
-        <v>20</v>
-      </c>
-      <c r="D22" s="37" t="s">
+      <c r="F21" s="23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="12">
+        <v>95</v>
+      </c>
+      <c r="D23" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E23" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="24" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="38" t="s">
+      <c r="F23" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="C24" s="32">
+        <v>70</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="12">
-        <v>95</v>
-      </c>
-      <c r="D24" s="35" t="s">
+      <c r="C26" s="32">
+        <v>50</v>
+      </c>
+      <c r="D26" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E26" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="42" t="s">
-        <v>322</v>
-      </c>
-      <c r="C25" s="34">
-        <v>70</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" s="23" t="s">
+      <c r="F26" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="12">
+        <v>4</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
-        <v>336</v>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="42" t="s">
+      <c r="F28" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="34">
-        <v>50</v>
-      </c>
-      <c r="D27" s="37" t="s">
+      <c r="C29" s="32">
+        <v>0</v>
+      </c>
+      <c r="D29" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="12">
-        <v>4</v>
-      </c>
-      <c r="D29" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="34">
-        <v>0</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="24" t="s">
+      <c r="F29" s="23" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C12" xr:uid="{E2FA9153-BF97-F44D-8444-660C47A52190}">
-      <formula1>1</formula1>
-      <formula2>10</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{BFC4374A-BF4E-D446-B591-ABBA5DFA0D32}">
+  <dataValidations count="8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{BFC4374A-BF4E-D446-B591-ABBA5DFA0D32}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29" xr:uid="{79437B14-BBCB-41C8-B199-9D1512AD30EC}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28" xr:uid="{79437B14-BBCB-41C8-B199-9D1512AD30EC}">
       <formula1>1</formula1>
       <formula2>52</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C21:C22 C27 C11:C12 C30 C24:C25 C18:C19 C14 C16" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C20:C21 C26 C10:C11 C29 C23:C24 C17:C18 C13" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{F1FF1A14-FBFD-4ABB-A983-0610B931ADEC}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{F1FF1A14-FBFD-4ABB-A983-0610B931ADEC}">
       <formula1>1</formula1>
       <formula2>21</formula2>
     </dataValidation>
@@ -7325,6 +7257,14 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{1FE2A73D-4B9A-994E-9090-48F33D0F77E3}">
+      <formula1>0</formula1>
+      <formula2>25</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C11" xr:uid="{E2FA9153-BF97-F44D-8444-660C47A52190}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add box to baseline
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCCB3DB-C493-C747-BE95-5ECE657D7EB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51ACBF2-0CDC-CA4A-B966-4BAF3F9CB28C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27100" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27100" windowHeight="17540" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="343">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1745,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1789,10 +1789,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1833,7 +1833,7 @@
         <v>43936</v>
       </c>
       <c r="D2" s="1">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>321</v>
@@ -1850,7 +1850,7 @@
         <v>44196</v>
       </c>
       <c r="D3" s="1">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>321</v>
@@ -1858,16 +1858,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B4" s="7">
-        <v>43866</v>
+        <v>43876</v>
       </c>
       <c r="C4" s="7">
-        <v>43890</v>
+        <v>43921</v>
       </c>
       <c r="D4" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>321</v>
@@ -1875,16 +1875,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>318</v>
       </c>
       <c r="B5" s="7">
-        <v>43891</v>
+        <v>43876</v>
       </c>
       <c r="C5" s="7">
-        <v>44012</v>
+        <v>43921</v>
       </c>
       <c r="D5" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>321</v>
@@ -1892,7 +1892,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>319</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -1901,7 +1901,7 @@
         <v>43921</v>
       </c>
       <c r="D6" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>321</v>
@@ -1909,50 +1909,50 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>318</v>
+        <v>98</v>
       </c>
       <c r="B7" s="7">
         <v>43876</v>
       </c>
       <c r="C7" s="7">
-        <v>43921</v>
+        <v>43936</v>
       </c>
       <c r="D7" s="1">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>319</v>
+        <v>98</v>
       </c>
       <c r="B8" s="7">
-        <v>43876</v>
+        <v>43937</v>
       </c>
       <c r="C8" s="7">
-        <v>43921</v>
+        <v>44196</v>
       </c>
       <c r="D8" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="B9" s="7">
         <v>43876</v>
       </c>
       <c r="C9" s="7">
-        <v>43936</v>
+        <v>43921</v>
       </c>
       <c r="D9" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>322</v>
@@ -1960,16 +1960,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>318</v>
       </c>
       <c r="B10" s="7">
-        <v>43937</v>
+        <v>43876</v>
       </c>
       <c r="C10" s="7">
-        <v>44196</v>
+        <v>43921</v>
       </c>
       <c r="D10" s="1">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>322</v>
@@ -1977,13 +1977,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>319</v>
       </c>
       <c r="B11" s="7">
-        <v>43866</v>
+        <v>43876</v>
       </c>
       <c r="C11" s="7">
-        <v>43890</v>
+        <v>43921</v>
       </c>
       <c r="D11" s="1">
         <v>50</v>
@@ -1994,16 +1994,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>320</v>
       </c>
       <c r="B12" s="7">
-        <v>43891</v>
+        <v>43876</v>
       </c>
       <c r="C12" s="7">
-        <v>44012</v>
+        <v>44196</v>
       </c>
       <c r="D12" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>322</v>
@@ -2011,16 +2011,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="B13" s="7">
-        <v>43876</v>
+        <v>43866</v>
       </c>
       <c r="C13" s="7">
-        <v>43921</v>
+        <v>43890</v>
       </c>
       <c r="D13" s="1">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>322</v>
@@ -2028,54 +2028,34 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>318</v>
+        <v>97</v>
       </c>
       <c r="B14" s="7">
-        <v>43876</v>
+        <v>43891</v>
       </c>
       <c r="C14" s="7">
-        <v>43921</v>
+        <v>44012</v>
       </c>
       <c r="D14" s="1">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B15" s="7">
-        <v>43876</v>
-      </c>
-      <c r="C15" s="7">
-        <v>43921</v>
-      </c>
-      <c r="D15" s="1">
-        <v>100</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B16" s="7">
-        <v>43876</v>
-      </c>
-      <c r="C16" s="7">
-        <v>44196</v>
-      </c>
-      <c r="D16" s="1">
-        <v>100</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
@@ -2287,37 +2267,9 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D46 D2:D8" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2330,13 +2282,13 @@
           <x14:formula1>
             <xm:f>HIDDEN!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E50</xm:sqref>
+          <xm:sqref>E2:E8 E9:E46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47936E1B-CEB7-1140-B286-248EE55FD596}">
           <x14:formula1>
             <xm:f>HIDDEN!$E$2:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A50</xm:sqref>
+          <xm:sqref>A2:A8 A9:A46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
adapt to different units
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1A15D-A0AA-D54C-BD47-A5B78BCF35CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123FB60-536A-B74C-86E8-C6D5DECDEC81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27100" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="-4160" yWindow="-19920" windowWidth="27100" windowHeight="17540" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="342">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1028,9 +1028,6 @@
     <t>Date End</t>
   </si>
   <si>
-    <t>Coverage (%)</t>
-  </si>
-  <si>
     <t>Maximum number of hospital surge beds</t>
   </si>
   <si>
@@ -1158,7 +1155,7 @@
     <t>Time to reach target coverage: (1 to 52)</t>
   </si>
   <si>
-    <t>Template v13.1</t>
+    <t>Template v13.2</t>
   </si>
 </sst>
 </file>
@@ -1745,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1756,7 +1753,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -1789,10 +1786,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1801,11 +1798,12 @@
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="8.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>310</v>
       </c>
@@ -1816,13 +1814,16 @@
         <v>313</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -1835,11 +1836,15 @@
       <c r="D2" s="1">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="str">
+        <f>IF(A2 = "", "", IF(A2="Screening (when S.I.)", "contacts", "%"))</f>
+        <v>%</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
@@ -1852,11 +1857,15 @@
       <c r="D3" s="1">
         <v>60</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="str">
+        <f t="shared" ref="E3:E46" si="0">IF(A3 = "", "", IF(A3="Screening (when S.I.)", "contacts", "%"))</f>
+        <v>%</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>137</v>
       </c>
@@ -1869,13 +1878,17 @@
       <c r="D4" s="1">
         <v>60</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B5" s="7">
         <v>43876</v>
@@ -1886,13 +1899,17 @@
       <c r="D5" s="1">
         <v>60</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>contacts</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -1903,11 +1920,15 @@
       <c r="D6" s="1">
         <v>50</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
@@ -1920,11 +1941,15 @@
       <c r="D7" s="1">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -1937,11 +1962,15 @@
       <c r="D8" s="1">
         <v>60</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>137</v>
       </c>
@@ -1954,13 +1983,17 @@
       <c r="D9" s="1">
         <v>60</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="7">
         <v>43876</v>
@@ -1971,13 +2004,17 @@
       <c r="D10" s="1">
         <v>60</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>contacts</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B11" s="7">
         <v>43876</v>
@@ -1988,13 +2025,17 @@
       <c r="D11" s="1">
         <v>50</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B12" s="7">
         <v>43876</v>
@@ -2005,11 +2046,15 @@
       <c r="D12" s="1">
         <v>100</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>97</v>
       </c>
@@ -2022,11 +2067,15 @@
       <c r="D13" s="1">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>97</v>
       </c>
@@ -2039,237 +2088,369 @@
       <c r="D14" s="1">
         <v>30</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>%</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F46" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D46 D2:D8" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D46" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2282,13 +2463,13 @@
           <x14:formula1>
             <xm:f>HIDDEN!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E8 E9:E46</xm:sqref>
+          <xm:sqref>F2:F46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47936E1B-CEB7-1140-B286-248EE55FD596}">
           <x14:formula1>
             <xm:f>HIDDEN!$E$2:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A8 A9:A46</xm:sqref>
+          <xm:sqref>A2:A46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2336,7 +2517,7 @@
         <v>137</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2347,10 +2528,10 @@
         <v>150</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2358,7 +2539,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2406,7 +2587,7 @@
         <v>157</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3151,7 +3332,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>128</v>
@@ -4294,7 +4475,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="170" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>134</v>
@@ -4568,7 +4749,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>129</v>
@@ -4959,7 +5140,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C4" s="1">
         <v>4.9000000000000002E-2</v>
@@ -5224,7 +5405,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" s="12">
         <v>3.5</v>
@@ -5241,7 +5422,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B4" s="12">
         <v>4.5</v>
@@ -5258,7 +5439,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
@@ -5290,7 +5471,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="12">
         <v>150</v>
@@ -5427,7 +5608,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B2" s="41">
         <v>160000</v>
@@ -5444,7 +5625,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B3" s="41">
         <v>8000</v>
@@ -5461,7 +5642,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" s="41">
         <v>8000</v>
@@ -5495,7 +5676,7 @@
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -5611,7 +5792,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -5628,7 +5809,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -5645,7 +5826,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -5692,8 +5873,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5757,7 +5938,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="30"/>
@@ -5768,7 +5949,7 @@
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C5" s="31">
         <v>4</v>
@@ -5784,7 +5965,7 @@
     <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C6" s="31">
         <v>80</v>
@@ -5796,12 +5977,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="30"/>
@@ -5830,7 +6011,7 @@
     <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="38" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C9" s="31">
         <v>2</v>
@@ -5922,7 +6103,7 @@
     <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C15" s="32">
         <v>5</v>
@@ -5934,7 +6115,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -6060,7 +6241,7 @@
     <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C24" s="32">
         <v>70</v>
@@ -6077,7 +6258,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" s="30"/>
@@ -6116,7 +6297,7 @@
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C28" s="12">
         <v>4</v>

</xml_diff>

<commit_message>
Update template, parameters range
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCEFD18-11C3-4840-ABE3-B7F991C0EB57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC61940-EB66-1A42-8808-F99BBD526DB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4160" yWindow="-19920" windowWidth="27100" windowHeight="17540" tabRatio="648" activeTab="7" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="2980" yWindow="460" windowWidth="24120" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="345">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1152,10 +1152,62 @@
     <t>Time to reach target coverage: (1 to 52)</t>
   </si>
   <si>
-    <t>Template v13.0</t>
-  </si>
-  <si>
-    <t>Scaling factor for infection hospitalisation rate: (1, 2, 3 or 4)</t>
+    <t>Template v13.0 B</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Scaling factor for infection hospitalisation rate: (0.1 to 5)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scaling factor for infection hospitalisation rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> accepted range of values is now 0.1 to 5.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Default value for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>handwashing efficacy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> set to 20%.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1166,7 +1218,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1211,6 +1263,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1343,7 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1422,9 +1482,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1740,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1774,6 +1831,21 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5575,8 +5647,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5674,9 +5746,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>341</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>342</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -5853,9 +5925,9 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{B4ABC229-799B-514E-B7F5-8FD96E5E9CBE}">
-      <formula1>1</formula1>
-      <formula2>4</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{B4ABC229-799B-514E-B7F5-8FD96E5E9CBE}">
+      <formula1>0.1</formula1>
+      <formula2>5</formula2>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{6C0631D2-5E94-0E44-AEDA-62F22487E25D}">
       <formula1>1</formula1>
@@ -5873,8 +5945,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6106,7 +6178,7 @@
         <v>327</v>
       </c>
       <c r="C15" s="32">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
update template to v14
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC61940-EB66-1A42-8808-F99BBD526DB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0CF978-3908-D44E-A837-673B20618BCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="460" windowWidth="24120" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="2640" yWindow="460" windowWidth="25280" windowHeight="17540" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="HIDDEN" sheetId="12" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="363">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1152,62 +1152,73 @@
     <t>Time to reach target coverage: (1 to 52)</t>
   </si>
   <si>
-    <t>Template v13.0 B</t>
-  </si>
-  <si>
-    <t>Changes</t>
-  </si>
-  <si>
     <t>Scaling factor for infection hospitalisation rate: (0.1 to 5)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Scaling factor for infection hospitalisation rate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> accepted range of values is now 0.1 to 5.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Default value for </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>handwashing efficacy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> set to 20%.</t>
-    </r>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>noise</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>Template v14</t>
+  </si>
+  <si>
+    <t>Minimum Age for vaccination</t>
+  </si>
+  <si>
+    <t>age_vaccine_min</t>
+  </si>
+  <si>
+    <t>Mass Testing</t>
+  </si>
+  <si>
+    <t>mass_test_sens</t>
+  </si>
+  <si>
+    <t>isolation_days</t>
+  </si>
+  <si>
+    <t>age_testing_min</t>
+  </si>
+  <si>
+    <t>age_testing_max</t>
+  </si>
+  <si>
+    <t>New in v14:</t>
+  </si>
+  <si>
+    <t>Isolation days</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Minimum age for mass testing (0 to 100)</t>
+  </si>
+  <si>
+    <t>Maximum age for mass testing (0 to 100)</t>
+  </si>
+  <si>
+    <t>Interventions sheet: added "Mass Testing" to the dropdown list of interventions.</t>
+  </si>
+  <si>
+    <t>Interventions Param sheet: Minimum Age for vaccination, 4 parameters for Mass Testing.</t>
+  </si>
+  <si>
+    <t>Parameters sheet: Iterations, Noise, Confidence.</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1229,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1270,15 +1281,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD0CECE"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1309,8 +1326,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1398,12 +1427,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1482,6 +1591,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1797,9 +1924,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1810,7 +1937,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -1835,17 +1962,22 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>344</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1861,7 +1993,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,7 +2029,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>308</v>
       </c>
       <c r="B2" s="7">
         <v>43876</v>
@@ -1909,7 +2041,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f>IF(A2 = "", "", IF(A2="Screening (when S.I.)", "contacts", "%"))</f>
+        <f>IF(A2 = "", "", IF(A2="Screening (when S.I.)", "contacts", IF(A2 = "Mass Testing", "tests", "%")))</f>
         <v>%</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1930,7 +2062,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E46" si="0">IF(A3 = "", "", IF(A3="Screening (when S.I.)", "contacts", "%"))</f>
+        <f t="shared" ref="E3:E46" si="0">IF(A3 = "", "", IF(A3="Screening (when S.I.)", "contacts", IF(A3 = "Mass Testing", "tests", "%")))</f>
         <v>%</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -2173,10 +2305,6 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2521,7 +2649,7 @@
       <c r="F46" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D46" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -2530,7 +2658,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{440D4135-AD3D-9D45-A472-9BA444A2B9DA}">
           <x14:formula1>
             <xm:f>HIDDEN!$G$2:$G$3</xm:f>
@@ -2539,7 +2667,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47936E1B-CEB7-1140-B286-248EE55FD596}">
           <x14:formula1>
-            <xm:f>HIDDEN!$E$2:$E$11</xm:f>
+            <xm:f>HIDDEN!$E$2:$E$12</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A46</xm:sqref>
         </x14:dataValidation>
@@ -2554,7 +2682,7 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2673,6 +2801,9 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>159</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5145,10 +5276,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5258,7 +5389,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>305</v>
       </c>
@@ -5273,6 +5404,56 @@
       </c>
       <c r="F7" s="14" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44">
+        <v>10</v>
+      </c>
+      <c r="D8" s="43"/>
+      <c r="E8" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54">
+        <v>5</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -5748,7 +5929,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -5943,10 +6124,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6384,26 +6565,126 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="39" t="s">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="C29" s="12">
+        <v>60</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="32">
-        <v>0</v>
-      </c>
-      <c r="D29" s="35" t="s">
+      <c r="C30" s="32">
+        <v>0</v>
+      </c>
+      <c r="D30" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E30" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F30" s="23" t="s">
         <v>125</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="C32" s="12">
+        <v>80</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="C33" s="12">
+        <v>14</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="C34" s="57">
+        <v>20</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="39" t="s">
+        <v>359</v>
+      </c>
+      <c r="C35" s="32">
+        <v>60</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{BFC4374A-BF4E-D446-B591-ABBA5DFA0D32}">
       <formula1>1</formula1>
       <formula2>5</formula2>
@@ -6412,7 +6693,7 @@
       <formula1>1</formula1>
       <formula2>52</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C20:C21 C26 C10:C11 C29 C23:C24 C17:C18 C13" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C20:C21 C26 C10:C11 C30 C23:C24 C17:C18 C13 C32 C33 C34 C35" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -6436,6 +6717,10 @@
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29" xr:uid="{B3A77258-E555-9644-BB0D-41361904BE89}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add barplot deaths by age category
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9429BF8-7ABF-4A4C-A953-204B95B18344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243E6804-1170-3340-8298-EBFED8AE0B21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="460" windowWidth="15540" windowHeight="17540" tabRatio="648" firstSheet="1" activeTab="5" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="12380" yWindow="460" windowWidth="15540" windowHeight="17540" tabRatio="648" firstSheet="1" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -5278,8 +5278,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5412,7 +5412,7 @@
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="44">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="45" t="s">
@@ -5497,7 +5497,7 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
mask wearing + dexamethanose
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A57219B-8103-5945-B2DE-901DB46F4F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863BA4C6-DAEC-FB4D-80E6-C9D5C6FA25DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="400">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -999,9 +999,6 @@
   </si>
   <si>
     <t>Shielding the Elderly</t>
-  </si>
-  <si>
-    <t>Interventions</t>
   </si>
   <si>
     <t>Intervention</t>
@@ -2027,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2038,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21">
@@ -2063,27 +2060,27 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="34">
       <c r="A10" s="49" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="34">
       <c r="A11" s="49" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="68">
       <c r="A12" s="49" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -2097,22 +2094,22 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2127,9 +2124,7 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2144,13 +2139,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17">
       <c r="A1" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>45</v>
@@ -2159,7 +2154,7 @@
         <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2180,7 +2175,7 @@
         <v>%</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2201,7 +2196,7 @@
         <v>%</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2222,12 +2217,12 @@
         <v>%</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B5" s="7">
         <v>43876</v>
@@ -2243,12 +2238,12 @@
         <v>contacts</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -2264,7 +2259,7 @@
         <v>%</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2285,7 +2280,7 @@
         <v>%</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2306,7 +2301,7 @@
         <v>%</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2327,12 +2322,12 @@
         <v>%</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B10" s="7">
         <v>43876</v>
@@ -2348,12 +2343,12 @@
         <v>contacts</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B11" s="7">
         <v>43876</v>
@@ -2369,12 +2364,12 @@
         <v>%</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B12" s="7">
         <v>43876</v>
@@ -2390,7 +2385,7 @@
         <v>%</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2411,12 +2406,12 @@
         <v>%</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B14" s="7">
         <v>43891</v>
@@ -2432,12 +2427,12 @@
         <v>tests</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B15" s="7">
         <v>43891</v>
@@ -2453,12 +2448,12 @@
         <v>%</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B16" s="7">
         <v>43910</v>
@@ -2474,7 +2469,7 @@
         <v>%</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2495,12 +2490,12 @@
         <v>%</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B18" s="7">
         <v>43983</v>
@@ -2516,7 +2511,7 @@
         <v>y.o.</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2861,7 +2856,7 @@
   <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2882,10 +2877,10 @@
         <v>305</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2902,7 +2897,7 @@
         <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2913,13 +2908,13 @@
         <v>146</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2927,7 +2922,7 @@
         <v>147</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>52</v>
@@ -2993,7 +2988,7 @@
         <v>153</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>52</v>
@@ -3015,7 +3010,7 @@
         <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>110</v>
@@ -3026,10 +3021,10 @@
         <v>156</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3037,7 +3032,7 @@
         <v>157</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>110</v>
@@ -3048,7 +3043,7 @@
         <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>110</v>
@@ -3059,7 +3054,7 @@
         <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>52</v>
@@ -3070,7 +3065,7 @@
         <v>160</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>52</v>
@@ -3081,7 +3076,7 @@
         <v>161</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -3783,7 +3778,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="68">
       <c r="A1" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>124</v>
@@ -4926,7 +4921,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="170">
       <c r="A1" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>130</v>
@@ -5200,7 +5195,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="68">
       <c r="A1" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>125</v>
@@ -5591,7 +5586,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" s="1">
         <v>4.9000000000000002E-2</v>
@@ -5656,7 +5651,7 @@
     </row>
     <row r="8" spans="1:6" s="46" customFormat="1">
       <c r="A8" s="43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="44">
@@ -5667,12 +5662,12 @@
         <v>47</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="46" customFormat="1">
       <c r="A9" s="43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="47">
@@ -5683,12 +5678,12 @@
         <v>47</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="46" customFormat="1">
       <c r="A10" s="43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="47">
@@ -5701,7 +5696,7 @@
         <v>47</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -5914,7 +5909,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3" s="12">
         <v>3.5</v>
@@ -5931,7 +5926,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="12">
         <v>4.5</v>
@@ -5948,7 +5943,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
@@ -5980,7 +5975,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B7" s="12">
         <v>150</v>
@@ -6048,7 +6043,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11" s="51">
         <v>50</v>
@@ -6060,7 +6055,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6134,7 +6129,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" s="41">
         <v>160000</v>
@@ -6151,7 +6146,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B3" s="41">
         <v>8000</v>
@@ -6168,7 +6163,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B4" s="41">
         <v>8000</v>
@@ -6202,7 +6197,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -6216,7 +6211,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="52" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B7" s="53">
         <v>35</v>
@@ -6233,7 +6228,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="52" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B8" s="53">
         <v>35</v>
@@ -6245,12 +6240,12 @@
         <v>47</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="52" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B9" s="53">
         <v>50</v>
@@ -6267,7 +6262,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B10" s="53">
         <v>50</v>
@@ -6279,12 +6274,12 @@
         <v>47</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="52" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B11" s="53">
         <v>55</v>
@@ -6301,7 +6296,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="52" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B12" s="53">
         <v>55</v>
@@ -6313,12 +6308,12 @@
         <v>47</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="52" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B13" s="53">
         <v>75</v>
@@ -6335,7 +6330,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="52" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14" s="53">
         <v>75</v>
@@ -6347,7 +6342,7 @@
         <v>47</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6386,7 +6381,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -6403,7 +6398,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -6420,7 +6415,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -6467,7 +6462,7 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -6532,7 +6527,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="30"/>
@@ -6543,7 +6538,7 @@
     <row r="5" spans="1:6" ht="17">
       <c r="A5" s="21"/>
       <c r="B5" s="38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" s="31">
         <v>4</v>
@@ -6559,7 +6554,7 @@
     <row r="6" spans="1:6" ht="18" thickBot="1">
       <c r="A6" s="21"/>
       <c r="B6" s="38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C6" s="31">
         <v>80</v>
@@ -6571,12 +6566,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="30"/>
@@ -6605,7 +6600,7 @@
     <row r="9" spans="1:6" ht="34">
       <c r="A9" s="18"/>
       <c r="B9" s="38" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C9" s="31">
         <v>2</v>
@@ -6697,7 +6692,7 @@
     <row r="15" spans="1:6" ht="18" thickBot="1">
       <c r="A15" s="24"/>
       <c r="B15" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C15" s="32">
         <v>20</v>
@@ -6709,12 +6704,12 @@
         <v>47</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="54" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B16" s="55"/>
       <c r="C16" s="56"/>
@@ -6725,7 +6720,7 @@
     <row r="17" spans="1:6" ht="18" thickBot="1">
       <c r="A17" s="65"/>
       <c r="B17" s="59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C17" s="67">
         <v>15</v>
@@ -6737,7 +6732,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6863,7 +6858,7 @@
     <row r="26" spans="1:6" ht="18" thickBot="1">
       <c r="A26" s="24"/>
       <c r="B26" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C26" s="32">
         <v>70</v>
@@ -6880,7 +6875,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B27" s="37"/>
       <c r="C27" s="30"/>
@@ -6919,7 +6914,7 @@
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="18"/>
       <c r="B30" s="36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C30" s="12">
         <v>4</v>
@@ -6937,7 +6932,7 @@
     <row r="31" spans="1:6" ht="17">
       <c r="A31" s="18"/>
       <c r="B31" s="36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C31" s="12">
         <v>60</v>
@@ -6949,7 +6944,7 @@
         <v>47</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" thickBot="1">
@@ -6972,7 +6967,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" s="30"/>
@@ -6983,7 +6978,7 @@
     <row r="34" spans="1:6" ht="17">
       <c r="A34" s="18"/>
       <c r="B34" s="36" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C34" s="12">
         <v>80</v>
@@ -6995,13 +6990,13 @@
         <v>47</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17">
       <c r="A35" s="18"/>
       <c r="B35" s="36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C35" s="12">
         <v>14</v>
@@ -7013,13 +7008,13 @@
         <v>47</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17">
       <c r="A36" s="18"/>
       <c r="B36" s="36" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C36" s="42">
         <v>20</v>
@@ -7031,13 +7026,13 @@
         <v>47</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1">
       <c r="A37" s="24"/>
       <c r="B37" s="39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C37" s="32">
         <v>60</v>
@@ -7049,12 +7044,12 @@
         <v>47</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="54" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B38" s="55"/>
       <c r="C38" s="56"/>
@@ -7065,7 +7060,7 @@
     <row r="39" spans="1:6" ht="34">
       <c r="A39" s="58"/>
       <c r="B39" s="59" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C39" s="60">
         <v>82</v>
@@ -7077,13 +7072,13 @@
         <v>47</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34">
       <c r="A40" s="52"/>
       <c r="B40" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C40" s="60">
         <v>64</v>
@@ -7095,13 +7090,13 @@
         <v>47</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="34">
       <c r="A41" s="58"/>
       <c r="B41" s="59" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C41" s="60">
         <v>82</v>
@@ -7113,13 +7108,13 @@
         <v>47</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="34">
       <c r="A42" s="58"/>
       <c r="B42" s="62" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C42" s="63">
         <v>64</v>
@@ -7131,13 +7126,13 @@
         <v>47</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" thickBot="1">
       <c r="A43" s="65"/>
       <c r="B43" s="66" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C43" s="67">
         <v>87</v>
@@ -7149,7 +7144,7 @@
         <v>47</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
max iterations noise set to 10,000
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ECC21C-F31F-2448-9EA5-A522A23AA727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E4BA1F-04EC-0E4A-8ECE-2ED42B7482DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="402">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -1191,9 +1191,6 @@
     <t>Minimum age for vaccination</t>
   </si>
   <si>
-    <t>Iterations (1 to 100)</t>
-  </si>
-  <si>
     <t>Noise (0.01 to 0.2)</t>
   </si>
   <si>
@@ -1203,9 +1200,6 @@
     <t>New in v15:</t>
   </si>
   <si>
-    <t>Template v15.2</t>
-  </si>
-  <si>
     <t>Proportion of hospitalised patients needing O2</t>
   </si>
   <si>
@@ -1291,29 +1285,6 @@
   </si>
   <si>
     <t>mask_eff</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">New in v15.2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>with changes compared to v15 in red in the sheets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t>Hospitalisation Param sheet: the four "Probability of dying ..." parameters are duplicated with (1) req O2 and (2) not req O2</t>
@@ -1351,6 +1322,21 @@
   <si>
     <t>Interventions: two interventions renamed: "(*Self-isolation) Screening" and 
 "(*Self-isolation) Household Isolation" and three options "(*Vaccination) Age Vaccine Minimum", "(*Mass Testing) Age Testing Minimum", "(*Mass Testing) Age Testing Maximum" added to allow overtime modification of these parameters.</t>
+  </si>
+  <si>
+    <t>Iterations (1 to 10,000)</t>
+  </si>
+  <si>
+    <t>Template v15.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New in v15.3 </t>
+  </si>
+  <si>
+    <t>Iterations can be set to 10,000 (previousely limit was 100)</t>
+  </si>
+  <si>
+    <t>New in v15.2:</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1347,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1427,9 +1413,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)_x0000_"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1569,7 +1558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1648,65 +1637,67 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2022,93 +2013,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="21">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="48" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="34">
-      <c r="A10" s="49" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="34">
-      <c r="A11" s="49" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="68">
-      <c r="A12" s="49" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="49"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="49"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="49"/>
-    </row>
-    <row r="17" spans="1:1">
+    <row r="8" spans="1:1" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="70" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="47" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="47" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="47"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="69" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
         <v>349</v>
       </c>
     </row>
@@ -2126,7 +2121,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
@@ -2137,7 +2132,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>305</v>
       </c>
@@ -2157,7 +2152,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2178,7 +2173,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -2199,7 +2194,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>133</v>
       </c>
@@ -2220,9 +2215,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B5" s="7">
         <v>43876</v>
@@ -2241,9 +2236,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -2262,7 +2257,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
@@ -2283,7 +2278,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>304</v>
       </c>
@@ -2304,7 +2299,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
@@ -2325,9 +2320,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B10" s="7">
         <v>43876</v>
@@ -2346,9 +2341,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B11" s="7">
         <v>43876</v>
@@ -2367,7 +2362,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>314</v>
       </c>
@@ -2388,7 +2383,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -2409,7 +2404,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>340</v>
       </c>
@@ -2430,9 +2425,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B15" s="7">
         <v>43891</v>
@@ -2451,9 +2446,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B16" s="7">
         <v>43910</v>
@@ -2472,7 +2467,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>119</v>
       </c>
@@ -2493,9 +2488,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B18" s="7">
         <v>43983</v>
@@ -2514,7 +2509,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2525,7 +2520,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2536,7 +2531,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2547,7 +2542,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2558,7 +2553,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2569,7 +2564,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2580,7 +2575,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -2591,7 +2586,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -2602,7 +2597,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -2613,7 +2608,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -2624,7 +2619,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -2635,7 +2630,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -2646,7 +2641,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -2657,7 +2652,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -2668,7 +2663,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -2679,7 +2674,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -2690,7 +2685,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -2701,7 +2696,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -2712,7 +2707,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -2723,7 +2718,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2734,7 +2729,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -2745,7 +2740,7 @@
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -2756,7 +2751,7 @@
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -2767,7 +2762,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -2778,7 +2773,7 @@
       </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2789,7 +2784,7 @@
       </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2800,7 +2795,7 @@
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -2811,7 +2806,7 @@
       </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2859,14 +2854,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
@@ -2877,13 +2872,13 @@
         <v>305</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="b">
         <v>0</v>
       </c>
@@ -2900,7 +2895,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
@@ -2908,27 +2903,27 @@
         <v>146</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>147</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>148</v>
       </c>
@@ -2939,7 +2934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>149</v>
       </c>
@@ -2950,7 +2945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>150</v>
       </c>
@@ -2961,7 +2956,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>151</v>
       </c>
@@ -2972,7 +2967,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>152</v>
       </c>
@@ -2983,7 +2978,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>153</v>
       </c>
@@ -2994,7 +2989,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
         <v>154</v>
       </c>
@@ -3005,18 +3000,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>156</v>
       </c>
@@ -3024,732 +3019,732 @@
         <v>340</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
         <v>160</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C18" s="2" t="s">
         <v>161</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="3:6">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="3:6">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="3:6">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="3:6">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="3:6">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="3:6">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="3:6">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="3:6">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="3:6">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="3:6">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="3:6">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="3:3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="3:3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="3:3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="3:3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="3:3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="3:3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="3:3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="3:3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="3:3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="3:3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="3:3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="3:3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="3:3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C69" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C71" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C73" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C75" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C77" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C80" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="81" spans="3:3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="3:3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="3:3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C83" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="3:3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C84" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="3:3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="3:3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="3:3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="3:3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="3:3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="3:3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="3:3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="3:3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="3:3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="3:3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="3:3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="3:3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="3:3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="3:3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="103" spans="3:3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="3:3">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="3:3">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="3:3">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="3:3">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="108" spans="3:3">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C108" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="3:3">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="3:3">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="3:3">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="112" spans="3:3">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C112" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="3:3">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="114" spans="3:3">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C114" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="115" spans="3:3">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="3:3">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C116" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="3:3">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="118" spans="3:3">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C118" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="119" spans="3:3">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C119" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="120" spans="3:3">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C120" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="121" spans="3:3">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C121" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="3:3">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C122" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="3:3">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="124" spans="3:3">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C124" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="125" spans="3:3">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C125" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="3:3">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C126" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="3:3">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C127" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="128" spans="3:3">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C128" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="129" spans="3:3">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="3:3">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="131" spans="3:3">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="132" spans="3:3">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="133" spans="3:3">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="134" spans="3:3">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="135" spans="3:3">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="136" spans="3:3">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="137" spans="3:3">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="138" spans="3:3">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="139" spans="3:3">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="140" spans="3:3">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="141" spans="3:3">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="142" spans="3:3">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="143" spans="3:3">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="144" spans="3:3">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="3:3">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="3:3">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="3:3">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="148" spans="3:3">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C148" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="149" spans="3:3">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C149" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="150" spans="3:3">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C150" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="151" spans="3:3">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C151" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="152" spans="3:3">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C152" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="153" spans="3:3">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C153" s="2" t="s">
         <v>296</v>
       </c>
@@ -3770,13 +3765,13 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11" style="1"/>
     <col min="4" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="68">
+    <row r="1" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>318</v>
       </c>
@@ -3787,7 +3782,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>43830</v>
       </c>
@@ -3798,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>43831</v>
       </c>
@@ -3809,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>43832</v>
       </c>
@@ -3820,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>43833</v>
       </c>
@@ -3831,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>43834</v>
       </c>
@@ -3842,7 +3837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>43835</v>
       </c>
@@ -3853,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>43836</v>
       </c>
@@ -3864,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43837</v>
       </c>
@@ -3875,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43838</v>
       </c>
@@ -3886,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43839</v>
       </c>
@@ -3897,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43840</v>
       </c>
@@ -3908,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>43841</v>
       </c>
@@ -3919,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>43842</v>
       </c>
@@ -3930,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43843</v>
       </c>
@@ -3941,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>43844</v>
       </c>
@@ -3952,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>43845</v>
       </c>
@@ -3963,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>43846</v>
       </c>
@@ -3974,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>43847</v>
       </c>
@@ -3985,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>43848</v>
       </c>
@@ -3996,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>43849</v>
       </c>
@@ -4007,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>43850</v>
       </c>
@@ -4018,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>43851</v>
       </c>
@@ -4029,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>43852</v>
       </c>
@@ -4040,7 +4035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>43853</v>
       </c>
@@ -4051,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>43854</v>
       </c>
@@ -4062,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>43855</v>
       </c>
@@ -4073,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>43856</v>
       </c>
@@ -4084,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>43857</v>
       </c>
@@ -4095,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>43858</v>
       </c>
@@ -4106,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>43859</v>
       </c>
@@ -4117,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>43860</v>
       </c>
@@ -4128,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>43861</v>
       </c>
@@ -4139,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>43862</v>
       </c>
@@ -4150,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>43863</v>
       </c>
@@ -4161,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>43864</v>
       </c>
@@ -4172,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>43865</v>
       </c>
@@ -4183,7 +4178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>43866</v>
       </c>
@@ -4194,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>43867</v>
       </c>
@@ -4205,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>43868</v>
       </c>
@@ -4216,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>43869</v>
       </c>
@@ -4227,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>43870</v>
       </c>
@@ -4238,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>43871</v>
       </c>
@@ -4249,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>43872</v>
       </c>
@@ -4260,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>43873</v>
       </c>
@@ -4271,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>43874</v>
       </c>
@@ -4282,7 +4277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>43875</v>
       </c>
@@ -4293,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>43876</v>
       </c>
@@ -4304,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>43877</v>
       </c>
@@ -4315,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>43878</v>
       </c>
@@ -4326,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>43879</v>
       </c>
@@ -4337,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>43880</v>
       </c>
@@ -4348,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>43881</v>
       </c>
@@ -4359,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>43882</v>
       </c>
@@ -4370,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>43883</v>
       </c>
@@ -4381,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>43884</v>
       </c>
@@ -4392,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>43885</v>
       </c>
@@ -4403,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>43886</v>
       </c>
@@ -4414,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>43887</v>
       </c>
@@ -4425,7 +4420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>43888</v>
       </c>
@@ -4436,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>43889</v>
       </c>
@@ -4447,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>43890</v>
       </c>
@@ -4458,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>43891</v>
       </c>
@@ -4469,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>43892</v>
       </c>
@@ -4480,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>43893</v>
       </c>
@@ -4491,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>43894</v>
       </c>
@@ -4502,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>43895</v>
       </c>
@@ -4513,7 +4508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>43896</v>
       </c>
@@ -4524,7 +4519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>43897</v>
       </c>
@@ -4535,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>43898</v>
       </c>
@@ -4546,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>43899</v>
       </c>
@@ -4557,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>43900</v>
       </c>
@@ -4568,7 +4563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>43901</v>
       </c>
@@ -4579,7 +4574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>43902</v>
       </c>
@@ -4590,7 +4585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>43903</v>
       </c>
@@ -4601,7 +4596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>43904</v>
       </c>
@@ -4612,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
         <v>43905</v>
       </c>
@@ -4623,7 +4618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>43906</v>
       </c>
@@ -4634,7 +4629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>43907</v>
       </c>
@@ -4645,7 +4640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>43908</v>
       </c>
@@ -4656,7 +4651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>43909</v>
       </c>
@@ -4667,7 +4662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>43910</v>
       </c>
@@ -4678,7 +4673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>43911</v>
       </c>
@@ -4689,7 +4684,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>43912</v>
       </c>
@@ -4700,7 +4695,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>43913</v>
       </c>
@@ -4711,7 +4706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>43914</v>
       </c>
@@ -4722,7 +4717,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>43915</v>
       </c>
@@ -4733,7 +4728,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>43916</v>
       </c>
@@ -4744,7 +4739,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>43917</v>
       </c>
@@ -4755,7 +4750,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>43918</v>
       </c>
@@ -4766,7 +4761,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>43919</v>
       </c>
@@ -4777,7 +4772,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>43920</v>
       </c>
@@ -4788,7 +4783,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>43921</v>
       </c>
@@ -4799,7 +4794,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>43922</v>
       </c>
@@ -4810,7 +4805,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>43923</v>
       </c>
@@ -4821,7 +4816,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>43924</v>
       </c>
@@ -4832,7 +4827,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>43925</v>
       </c>
@@ -4843,7 +4838,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>43926</v>
       </c>
@@ -4854,37 +4849,37 @@
         <v>708</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>43927</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>43928</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>43929</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>43930</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>43931</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>43932</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>43933</v>
       </c>
@@ -4911,7 +4906,7 @@
       <selection activeCell="C22" sqref="B2:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="8" customWidth="1"/>
@@ -4919,7 +4914,7 @@
     <col min="4" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="170">
+    <row r="1" spans="1:3" ht="170" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>317</v>
       </c>
@@ -4930,7 +4925,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -4941,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -4952,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -4963,7 +4958,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -4974,7 +4969,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -4985,7 +4980,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -4996,7 +4991,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -5018,7 +5013,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -5029,7 +5024,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -5040,7 +5035,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -5051,7 +5046,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -5062,7 +5057,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -5073,7 +5068,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
@@ -5084,7 +5079,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
@@ -5095,7 +5090,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -5106,7 +5101,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
@@ -5117,7 +5112,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
@@ -5128,7 +5123,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
@@ -5139,7 +5134,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -5150,7 +5145,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -5183,7 +5178,7 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="10" bestFit="1" customWidth="1"/>
@@ -5193,7 +5188,7 @@
     <col min="7" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="68">
+    <row r="1" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>317</v>
       </c>
@@ -5207,7 +5202,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
@@ -5221,7 +5216,7 @@
         <v>2.3722458400227202E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
@@ -5235,7 +5230,7 @@
         <v>1.32905378016121E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
@@ -5249,7 +5244,7 @@
         <v>2.7683021103459102E-7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -5263,7 +5258,7 @@
         <v>5.9421612308889897E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
@@ -5277,7 +5272,7 @@
         <v>9.4061131337053795E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
@@ -5291,7 +5286,7 @@
         <v>1.22116449024625E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>28</v>
       </c>
@@ -5305,7 +5300,7 @@
         <v>1.74496544750293E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
@@ -5319,7 +5314,7 @@
         <v>2.3869666845092401E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
@@ -5333,7 +5328,7 @@
         <v>3.9402680780452703E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
@@ -5347,7 +5342,7 @@
         <v>5.9906418526633501E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -5361,7 +5356,7 @@
         <v>8.5059441930317695E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
@@ -5375,7 +5370,7 @@
         <v>1.26668575743058E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>2.0472533414662599E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
@@ -5403,7 +5398,7 @@
         <v>3.4000512436294603E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>36</v>
       </c>
@@ -5417,7 +5412,7 @@
         <v>4.9617484749088298E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>37</v>
       </c>
@@ -5431,7 +5426,7 @@
         <v>8.7449779441565906E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>38</v>
       </c>
@@ -5445,7 +5440,7 @@
         <v>1.6171761126065301E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>39</v>
       </c>
@@ -5459,7 +5454,7 @@
         <v>2.9461103089733202E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>40</v>
       </c>
@@ -5473,7 +5468,7 @@
         <v>4.9738551978041395E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>41</v>
       </c>
@@ -5487,7 +5482,7 @@
         <v>8.9717264255251901E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>20</v>
       </c>
@@ -5522,10 +5517,10 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.33203125" style="8" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
@@ -5536,7 +5531,7 @@
     <col min="7" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -5556,7 +5551,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>134</v>
       </c>
@@ -5570,7 +5565,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>135</v>
       </c>
@@ -5584,7 +5579,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>323</v>
       </c>
@@ -5598,7 +5593,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>302</v>
       </c>
@@ -5615,7 +5610,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>303</v>
       </c>
@@ -5632,7 +5627,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>301</v>
       </c>
@@ -5649,53 +5644,53 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="46" customFormat="1">
-      <c r="A8" s="43" t="s">
+    <row r="8" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43">
+        <v>1</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="42" t="s">
         <v>353</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44">
-        <v>1</v>
-      </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="45" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="45" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="46" customFormat="1">
-      <c r="A9" s="43" t="s">
+      <c r="F9" s="44" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="47">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="45" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="46">
+        <v>5</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="45" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="46" customFormat="1">
-      <c r="A10" s="43" t="s">
-        <v>355</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="47">
-        <v>5</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="44" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5722,7 +5717,7 @@
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{CB814818-B5CA-A746-A079-0D54DE38C760}">
       <formula1>1</formula1>
-      <formula2>100</formula2>
+      <formula2>10000</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{86EA7129-76D5-C14C-A270-6059C886D569}">
       <formula1>0.01</formula1>
@@ -5744,7 +5739,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" style="8" bestFit="1" customWidth="1"/>
@@ -5755,7 +5750,7 @@
     <col min="7" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -5775,7 +5770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>297</v>
       </c>
@@ -5791,7 +5786,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -5808,7 +5803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>57</v>
       </c>
@@ -5859,10 +5854,10 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53.5" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -5873,7 +5868,7 @@
     <col min="8" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -5890,7 +5885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
         <v>55</v>
       </c>
@@ -5907,7 +5902,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="40" t="s">
         <v>324</v>
       </c>
@@ -5924,7 +5919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="40" t="s">
         <v>325</v>
       </c>
@@ -5941,7 +5936,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>326</v>
       </c>
@@ -5956,7 +5951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
         <v>62</v>
       </c>
@@ -5973,7 +5968,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
         <v>327</v>
       </c>
@@ -5990,7 +5985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="40" t="s">
         <v>66</v>
       </c>
@@ -6007,7 +6002,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
         <v>68</v>
       </c>
@@ -6024,7 +6019,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>70</v>
       </c>
@@ -6041,21 +6036,21 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="50" t="s">
-        <v>358</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>356</v>
       </c>
       <c r="B11" s="51">
         <v>50</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -6097,10 +6092,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="8" bestFit="1" customWidth="1"/>
@@ -6110,7 +6105,7 @@
     <col min="6" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -6127,7 +6122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>309</v>
       </c>
@@ -6144,7 +6139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>310</v>
       </c>
@@ -6161,7 +6156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>311</v>
       </c>
@@ -6178,7 +6173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>132</v>
       </c>
@@ -6195,7 +6190,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>335</v>
       </c>
@@ -6209,14 +6204,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="52" t="s">
-        <v>361</v>
-      </c>
-      <c r="B7" s="53">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B7" s="6">
         <v>35</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -6226,31 +6221,31 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="52" t="s">
-        <v>362</v>
-      </c>
-      <c r="B8" s="53">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" s="6">
         <v>35</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="52" t="s">
-        <v>364</v>
-      </c>
-      <c r="B9" s="53">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="6">
         <v>50</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -6260,31 +6255,31 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="52" t="s">
-        <v>365</v>
-      </c>
-      <c r="B10" s="53">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" s="6">
         <v>50</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="52" t="s">
-        <v>367</v>
-      </c>
-      <c r="B11" s="53">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B11" s="6">
         <v>55</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -6294,31 +6289,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="52" t="s">
-        <v>368</v>
-      </c>
-      <c r="B12" s="53">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B12" s="6">
         <v>55</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="B13" s="53">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="B13" s="6">
         <v>75</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -6328,24 +6323,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="B14" s="53">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="B14" s="6">
         <v>75</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>85</v>
       </c>
@@ -6362,7 +6357,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>86</v>
       </c>
@@ -6379,7 +6374,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>328</v>
       </c>
@@ -6396,7 +6391,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>329</v>
       </c>
@@ -6413,7 +6408,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>330</v>
       </c>
@@ -6462,11 +6457,11 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" style="8" customWidth="1"/>
@@ -6477,7 +6472,7 @@
     <col min="7" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>91</v>
       </c>
@@ -6497,7 +6492,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>133</v>
       </c>
@@ -6507,7 +6502,7 @@
       <c r="E2" s="28"/>
       <c r="F2" s="29"/>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1">
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="36" t="s">
         <v>102</v>
@@ -6525,7 +6520,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>312</v>
       </c>
@@ -6535,7 +6530,7 @@
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
     </row>
-    <row r="5" spans="1:6" ht="17">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="38" t="s">
         <v>331</v>
@@ -6551,7 +6546,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1">
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="38" t="s">
         <v>319</v>
@@ -6569,7 +6564,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>313</v>
       </c>
@@ -6579,7 +6574,7 @@
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="36" t="s">
         <v>116</v>
@@ -6597,7 +6592,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="38" t="s">
         <v>332</v>
@@ -6615,7 +6610,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>117</v>
@@ -6633,7 +6628,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="35" thickBot="1">
+    <row r="11" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="39" t="s">
         <v>118</v>
@@ -6651,25 +6646,25 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="34"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="28"/>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:6" ht="18" thickBot="1">
-      <c r="A13" s="24"/>
-      <c r="B13" s="39" t="s">
+    <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
+      <c r="B13" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="58">
         <v>100</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E13" s="22" t="s">
@@ -6679,25 +6674,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="34"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
       <c r="E14" s="28"/>
       <c r="F14" s="29"/>
     </row>
-    <row r="15" spans="1:6" ht="18" thickBot="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="56"/>
+      <c r="B15" s="60" t="s">
         <v>322</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="58">
         <v>20</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -6707,53 +6702,53 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="54" t="s">
-        <v>384</v>
-      </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
     </row>
-    <row r="17" spans="1:6" ht="18" thickBot="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="59" t="s">
-        <v>385</v>
-      </c>
-      <c r="C17" s="67">
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="56"/>
+      <c r="B17" s="61" t="s">
+        <v>383</v>
+      </c>
+      <c r="C17" s="62">
         <v>15</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="34"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="28"/>
       <c r="F18" s="29"/>
     </row>
-    <row r="19" spans="1:6" ht="17">
-      <c r="A19" s="18"/>
-      <c r="B19" s="36" t="s">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="63"/>
+      <c r="B19" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="51">
         <v>85</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="64" t="s">
         <v>52</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -6763,15 +6758,15 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="35" thickBot="1">
-      <c r="A20" s="24"/>
-      <c r="B20" s="39" t="s">
+    <row r="20" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="58">
         <v>10</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="22" t="s">
@@ -6781,25 +6776,25 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="25" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="34"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="28"/>
       <c r="F21" s="29"/>
     </row>
-    <row r="22" spans="1:6" ht="17">
-      <c r="A22" s="18"/>
-      <c r="B22" s="36" t="s">
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="63"/>
+      <c r="B22" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="51">
         <v>85</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="64" t="s">
         <v>52</v>
       </c>
       <c r="E22" s="19" t="s">
@@ -6809,15 +6804,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" thickBot="1">
-      <c r="A23" s="24"/>
-      <c r="B23" s="39" t="s">
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
+      <c r="B23" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="58">
         <v>20</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="22" t="s">
@@ -6827,25 +6822,25 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
         <v>304</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="28"/>
       <c r="F24" s="29"/>
     </row>
-    <row r="25" spans="1:6" ht="17">
-      <c r="A25" s="18"/>
-      <c r="B25" s="36" t="s">
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="63"/>
+      <c r="B25" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="51">
         <v>95</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="64" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="19" t="s">
@@ -6855,15 +6850,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" thickBot="1">
-      <c r="A26" s="24"/>
-      <c r="B26" s="39" t="s">
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="57" t="s">
         <v>333</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="58">
         <v>70</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="59" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="22" t="s">
@@ -6873,25 +6868,25 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="25" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
         <v>314</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="34"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="28"/>
       <c r="F27" s="29"/>
     </row>
-    <row r="28" spans="1:6" ht="18" thickBot="1">
-      <c r="A28" s="24"/>
-      <c r="B28" s="39" t="s">
+    <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="56"/>
+      <c r="B28" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="58">
         <v>50</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="22" t="s">
@@ -6901,25 +6896,25 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="34"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="28"/>
       <c r="F29" s="29"/>
     </row>
-    <row r="30" spans="1:6" ht="17">
-      <c r="A30" s="18"/>
-      <c r="B30" s="36" t="s">
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="63"/>
+      <c r="B30" s="60" t="s">
         <v>334</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="51">
         <v>4</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="64" t="s">
         <v>98</v>
       </c>
       <c r="E30" s="19" t="s">
@@ -6929,15 +6924,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17">
-      <c r="A31" s="18"/>
-      <c r="B31" s="36" t="s">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="63"/>
+      <c r="B31" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="51">
         <v>60</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="64" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="19" t="s">
@@ -6947,15 +6942,15 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" thickBot="1">
-      <c r="A32" s="24"/>
-      <c r="B32" s="39" t="s">
+    <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="32">
-        <v>0</v>
-      </c>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="58">
+        <v>0</v>
+      </c>
+      <c r="D32" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E32" s="22" t="s">
@@ -6965,25 +6960,25 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="25" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="52" t="s">
         <v>340</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="28"/>
       <c r="F33" s="29"/>
     </row>
-    <row r="34" spans="1:6" ht="17">
-      <c r="A34" s="18"/>
-      <c r="B34" s="36" t="s">
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="63"/>
+      <c r="B34" s="60" t="s">
         <v>346</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="51">
         <v>80</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="64" t="s">
         <v>52</v>
       </c>
       <c r="E34" s="19" t="s">
@@ -6993,15 +6988,15 @@
         <v>341</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17">
-      <c r="A35" s="18"/>
-      <c r="B35" s="36" t="s">
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="63"/>
+      <c r="B35" s="60" t="s">
         <v>345</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="51">
         <v>14</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="64" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="19" t="s">
@@ -7011,15 +7006,15 @@
         <v>342</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17">
-      <c r="A36" s="18"/>
-      <c r="B36" s="36" t="s">
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="63"/>
+      <c r="B36" s="60" t="s">
         <v>347</v>
       </c>
-      <c r="C36" s="42">
+      <c r="C36" s="65">
         <v>20</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="64" t="s">
         <v>110</v>
       </c>
       <c r="E36" s="19" t="s">
@@ -7029,15 +7024,15 @@
         <v>343</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="39" t="s">
+    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56"/>
+      <c r="B37" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="58">
         <v>60</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="59" t="s">
         <v>110</v>
       </c>
       <c r="E37" s="22" t="s">
@@ -7047,76 +7042,76 @@
         <v>344</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="54" t="s">
-        <v>373</v>
-      </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="57"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="52" t="s">
+        <v>371</v>
+      </c>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="28"/>
       <c r="F38" s="29"/>
     </row>
-    <row r="39" spans="1:6" ht="34">
-      <c r="A39" s="58"/>
-      <c r="B39" s="59" t="s">
-        <v>374</v>
-      </c>
-      <c r="C39" s="60">
+    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="63"/>
+      <c r="B39" s="61" t="s">
+        <v>372</v>
+      </c>
+      <c r="C39" s="66">
         <v>82</v>
       </c>
-      <c r="D39" s="61" t="s">
+      <c r="D39" s="67" t="s">
         <v>52</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="34">
-      <c r="A40" s="52"/>
-      <c r="B40" s="59" t="s">
-        <v>376</v>
-      </c>
-      <c r="C40" s="60">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="C40" s="66">
         <v>64</v>
       </c>
-      <c r="D40" s="61" t="s">
+      <c r="D40" s="67" t="s">
         <v>52</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="34">
-      <c r="A41" s="58"/>
-      <c r="B41" s="59" t="s">
-        <v>378</v>
-      </c>
-      <c r="C41" s="60">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="63"/>
+      <c r="B41" s="61" t="s">
+        <v>376</v>
+      </c>
+      <c r="C41" s="66">
         <v>82</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="67" t="s">
         <v>52</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>47</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="34">
-      <c r="A42" s="58"/>
-      <c r="B42" s="62" t="s">
-        <v>380</v>
-      </c>
-      <c r="C42" s="63">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="63"/>
+      <c r="B42" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="C42" s="68">
         <v>64</v>
       </c>
       <c r="D42" s="64" t="s">
@@ -7126,25 +7121,25 @@
         <v>47</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18" thickBot="1">
-      <c r="A43" s="65"/>
-      <c r="B43" s="66" t="s">
-        <v>382</v>
-      </c>
-      <c r="C43" s="67">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="57" t="s">
+        <v>380</v>
+      </c>
+      <c r="C43" s="62">
         <v>87</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="59" t="s">
         <v>52</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple modifs for v16.2
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2C6FE-30A4-CC42-B992-CBA317E78FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D256327C-DCE5-644F-B846-4D93A8446C25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1280" windowWidth="26960" windowHeight="21000" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="-38400" yWindow="-1280" windowWidth="26960" windowHeight="21000" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1149,9 +1149,6 @@
     <t>dexv</t>
   </si>
   <si>
-    <t>Relative risk of dying if needing  but not receivingO2 and taking Dex</t>
-  </si>
-  <si>
     <t>dexo2c</t>
   </si>
   <si>
@@ -2822,6 +2819,9 @@
       </rPr>
       <t xml:space="preserve"> Mass Testing unit is now thousand tests allowing to perform up to 100,000 tests.</t>
     </r>
+  </si>
+  <si>
+    <t>Relative risk of dying if needing  but not receiving O2 and taking Dex</t>
   </si>
 </sst>
 </file>
@@ -3591,7 +3591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3602,7 +3602,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21">
@@ -3627,47 +3627,47 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="59" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="34">
       <c r="A8" s="38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="17">
       <c r="A9" s="38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="17">
       <c r="A10" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="17">
       <c r="A11" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="34">
       <c r="A12" s="38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="84" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="39" customFormat="1">
       <c r="A15" s="40" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="85" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -3677,17 +3677,17 @@
     </row>
     <row r="19" spans="1:1" ht="34">
       <c r="A19" s="38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="34">
       <c r="A20" s="38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="68">
       <c r="A21" s="38" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -3695,7 +3695,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="85" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -3825,7 +3825,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B5" s="7">
         <v>43876</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B6" s="7">
         <v>43876</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B10" s="7">
         <v>43876</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B11" s="7">
         <v>43876</v>
@@ -4035,7 +4035,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B15" s="7">
         <v>43891</v>
@@ -4098,7 +4098,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B18" s="7">
         <v>43983</v>
@@ -4119,7 +4119,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B19" s="7">
         <v>43983</v>
@@ -4490,7 +4490,7 @@
         <v>292</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>293</v>
@@ -4521,10 +4521,10 @@
         <v>137</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>301</v>
@@ -4535,7 +4535,7 @@
         <v>138</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>52</v>
@@ -4623,7 +4623,7 @@
         <v>146</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>103</v>
@@ -4634,7 +4634,7 @@
         <v>147</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>103</v>
@@ -4648,7 +4648,7 @@
         <v>319</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -4656,7 +4656,7 @@
         <v>149</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>103</v>
@@ -4667,7 +4667,7 @@
         <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>103</v>
@@ -4678,7 +4678,7 @@
         <v>151</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>52</v>
@@ -4700,7 +4700,7 @@
         <v>153</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="3:6">
@@ -7177,7 +7177,7 @@
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="64" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B2" s="62">
         <v>43862</v>
@@ -7193,7 +7193,7 @@
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="64" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B3" s="62">
         <v>44196</v>
@@ -7209,7 +7209,7 @@
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" s="64" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="70">
@@ -7220,12 +7220,12 @@
         <v>44</v>
       </c>
       <c r="F4" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="73" customFormat="1" ht="17">
       <c r="A5" s="64" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B5" s="69"/>
       <c r="C5" s="71">
@@ -7238,12 +7238,12 @@
         <v>47</v>
       </c>
       <c r="F5" s="67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="64" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B6" s="61"/>
       <c r="C6" s="63">
@@ -7259,7 +7259,7 @@
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="64" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B7" s="61"/>
       <c r="C7" s="63">
@@ -7277,7 +7277,7 @@
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B8" s="61"/>
       <c r="C8" s="63">
@@ -7295,7 +7295,7 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="64" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="63">
@@ -7308,12 +7308,12 @@
         <v>47</v>
       </c>
       <c r="F9" s="67" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34">
       <c r="A10" s="64" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B10" s="61"/>
       <c r="C10" s="63">
@@ -7331,7 +7331,7 @@
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="64" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="63">
@@ -7344,12 +7344,12 @@
         <v>47</v>
       </c>
       <c r="F11" s="67" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34">
       <c r="A12" s="64" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="63">
@@ -7362,12 +7362,12 @@
         <v>47</v>
       </c>
       <c r="F12" s="67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34">
       <c r="A13" s="64" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B13" s="61"/>
       <c r="C13" s="63">
@@ -7380,12 +7380,12 @@
         <v>47</v>
       </c>
       <c r="F13" s="67" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34">
       <c r="A14" s="64" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B14" s="61"/>
       <c r="C14" s="63">
@@ -7398,12 +7398,12 @@
         <v>47</v>
       </c>
       <c r="F14" s="67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34">
       <c r="A15" s="64" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="61"/>
       <c r="C15" s="63">
@@ -7416,12 +7416,12 @@
         <v>47</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34">
       <c r="A16" s="64" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B16" s="61"/>
       <c r="C16" s="63">
@@ -7434,12 +7434,12 @@
         <v>47</v>
       </c>
       <c r="F16" s="67" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34">
       <c r="A17" s="64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B17" s="61"/>
       <c r="C17" s="63">
@@ -7452,12 +7452,12 @@
         <v>47</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="64" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B18" s="61"/>
       <c r="C18" s="63">
@@ -7470,12 +7470,12 @@
         <v>47</v>
       </c>
       <c r="F18" s="67" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34">
       <c r="A19" s="64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B19" s="61"/>
       <c r="C19" s="63">
@@ -7488,12 +7488,12 @@
         <v>47</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34">
       <c r="A20" s="64" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B20" s="61"/>
       <c r="C20" s="63">
@@ -7506,12 +7506,12 @@
         <v>47</v>
       </c>
       <c r="F20" s="67" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
       <c r="A21" s="72" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B21" s="65"/>
       <c r="C21" s="66">
@@ -7641,7 +7641,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>277</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C3" s="1">
         <v>2.8</v>
@@ -7674,7 +7674,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -7756,7 +7756,7 @@
     </row>
     <row r="2" spans="1:5" ht="17">
       <c r="A2" s="75" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B2" s="77">
         <v>10</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="3" spans="1:5" ht="17">
       <c r="A3" s="75" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B3" s="77">
         <v>3.5</v>
@@ -7790,7 +7790,7 @@
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="75" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B4" s="77">
         <v>4.5</v>
@@ -7807,7 +7807,7 @@
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B5" s="77">
         <v>1</v>
@@ -7822,7 +7822,7 @@
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="75" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B6" s="77">
         <v>0</v>
@@ -7839,7 +7839,7 @@
     </row>
     <row r="7" spans="1:5" ht="17">
       <c r="A7" s="75" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B7" s="77">
         <v>150</v>
@@ -7856,7 +7856,7 @@
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="75" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B8" s="77">
         <v>55</v>
@@ -7873,7 +7873,7 @@
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B9" s="77">
         <v>50</v>
@@ -7890,7 +7890,7 @@
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="75" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B10" s="77">
         <v>75</v>
@@ -7924,7 +7924,7 @@
     </row>
     <row r="12" spans="1:5" ht="34">
       <c r="A12" s="75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B12" s="79">
         <v>50</v>
@@ -7936,12 +7936,12 @@
         <v>47</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="34">
       <c r="A13" s="75" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B13" s="79">
         <v>50</v>
@@ -7953,12 +7953,12 @@
         <v>47</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="34">
       <c r="A14" s="75" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B14" s="79">
         <v>50</v>
@@ -7970,12 +7970,12 @@
         <v>47</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34">
       <c r="A15" s="75" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B15" s="79">
         <v>50</v>
@@ -7987,12 +7987,12 @@
         <v>47</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="34">
       <c r="A16" s="75" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B16" s="79">
         <v>50</v>
@@ -8004,12 +8004,12 @@
         <v>47</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34">
       <c r="A17" s="75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B17" s="79">
         <v>50</v>
@@ -8021,12 +8021,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
       <c r="A18" s="75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B18" s="79">
         <v>50</v>
@@ -8038,12 +8038,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
       <c r="A19" s="75" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B19" s="79">
         <v>50</v>
@@ -8055,12 +8055,12 @@
         <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A20" s="75" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B20" s="81">
         <v>50</v>
@@ -8072,12 +8072,12 @@
         <v>47</v>
       </c>
       <c r="E20" s="82" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A21" s="76" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B21" s="81">
         <v>0</v>
@@ -8089,12 +8089,12 @@
         <v>47</v>
       </c>
       <c r="E21" s="82" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="74" customFormat="1" ht="17" customHeight="1">
       <c r="A22" s="75" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B22" s="81">
         <v>100</v>
@@ -8106,12 +8106,12 @@
         <v>47</v>
       </c>
       <c r="E22" s="82" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="74" customFormat="1" ht="17" customHeight="1">
       <c r="A23" s="75" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B23" s="81">
         <v>100</v>
@@ -8123,12 +8123,12 @@
         <v>47</v>
       </c>
       <c r="E23" s="82" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A24" s="75" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B24" s="81">
         <v>100</v>
@@ -8140,12 +8140,12 @@
         <v>47</v>
       </c>
       <c r="E24" s="82" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="74" customFormat="1" ht="17">
       <c r="A25" s="75" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B25" s="81">
         <v>100</v>
@@ -8157,7 +8157,7 @@
         <v>47</v>
       </c>
       <c r="E25" s="82" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -8495,7 +8495,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B17">
         <v>95</v>
@@ -8507,12 +8507,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B18">
         <v>95</v>
@@ -8524,12 +8524,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B19">
         <v>95</v>
@@ -8541,7 +8541,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -8627,8 +8627,8 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -8692,7 +8692,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="27"/>
@@ -8736,7 +8736,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="34"/>
       <c r="C7" s="27"/>
@@ -8874,7 +8874,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="42" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="44"/>
@@ -8885,7 +8885,7 @@
     <row r="17" spans="1:6" ht="18" thickBot="1">
       <c r="A17" s="46"/>
       <c r="B17" s="51" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C17" s="52">
         <v>15</v>
@@ -8897,7 +8897,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -9079,7 +9079,7 @@
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="53"/>
       <c r="B30" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C30" s="41">
         <v>4</v>
@@ -9115,7 +9115,7 @@
     <row r="32" spans="1:6" ht="17">
       <c r="A32" s="53"/>
       <c r="B32" s="33" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C32" s="11">
         <v>100</v>
@@ -9127,13 +9127,13 @@
         <v>47</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17">
       <c r="A33" s="53"/>
       <c r="B33" s="33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C33" s="11">
         <v>100</v>
@@ -9145,13 +9145,13 @@
         <v>47</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34">
       <c r="A34" s="53"/>
       <c r="B34" s="33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C34" s="11">
         <v>100</v>
@@ -9163,13 +9163,13 @@
         <v>47</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17">
       <c r="A35" s="53"/>
       <c r="B35" s="33" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C35" s="83">
         <v>100</v>
@@ -9187,7 +9187,7 @@
     <row r="36" spans="1:6" ht="18" thickBot="1">
       <c r="A36" s="46"/>
       <c r="B36" s="36" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C36" s="29">
         <v>100</v>
@@ -9199,7 +9199,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -9333,7 +9333,7 @@
     <row r="45" spans="1:6" ht="34">
       <c r="A45" s="53"/>
       <c r="B45" s="51" t="s">
-        <v>354</v>
+        <v>475</v>
       </c>
       <c r="C45" s="56">
         <v>82</v>
@@ -9345,13 +9345,13 @@
         <v>47</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="34">
       <c r="A46" s="53"/>
       <c r="B46" s="50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C46" s="58">
         <v>64</v>
@@ -9363,13 +9363,13 @@
         <v>47</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1">
       <c r="A47" s="46"/>
       <c r="B47" s="47" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C47" s="52">
         <v>87</v>
@@ -9381,7 +9381,7 @@
         <v>47</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increase limit to 50 interventions
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A85F0E-8BF5-D749-A8C7-469404B70AD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B47780-84A7-3941-B54D-5446CC0CC764}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="477">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -2821,6 +2821,9 @@
   </si>
   <si>
     <t>Relative risk of dying if needing  but not receiving O2 and taking Dex</t>
+  </si>
+  <si>
+    <t>(There is a maximum of 50 interventions in this version).</t>
   </si>
 </sst>
 </file>
@@ -3590,7 +3593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3722,10 +3725,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4434,9 +4437,69 @@
       </c>
       <c r="F46" s="1"/>
     </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2" t="str">
+        <f>IF(A47="","",VLOOKUP(A47,HIDDEN!$E$2:$F$18,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2" t="str">
+        <f>IF(A48="","",VLOOKUP(A48,HIDDEN!$E$2:$F$18,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2" t="str">
+        <f>IF(A49="","",VLOOKUP(A49,HIDDEN!$E$2:$F$18,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2" t="str">
+        <f>IF(A50="","",VLOOKUP(A50,HIDDEN!$E$2:$F$18,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2" t="str">
+        <f>IF(A51="","",VLOOKUP(A51,HIDDEN!$E$2:$F$18,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D46" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D51" xr:uid="{D6E5BF00-5D2D-744A-810E-E4B5BEB9445C}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -4449,13 +4512,13 @@
           <x14:formula1>
             <xm:f>HIDDEN!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F46</xm:sqref>
+          <xm:sqref>F2:F51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8111968A-8FE9-DE4F-AE93-5F28872C16C3}">
           <x14:formula1>
             <xm:f>HIDDEN!$E$2:$E$18</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A46</xm:sqref>
+          <xm:sqref>A2:A51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update table param report
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40347114-5ADE-5747-8E9C-38335337BDCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3945FA62-DC25-D749-A704-1032EFFEEA65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3593,7 +3593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -3725,7 +3725,7 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -7192,7 +7192,9 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -7655,7 +7657,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -7772,7 +7774,9 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -8258,7 +8262,9 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>

</xml_diff>

<commit_message>
replace reporth_g with report_g
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3945FA62-DC25-D749-A704-1032EFFEEA65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79C95D-7329-B544-98C2-F966C2A2406A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -1221,9 +1221,6 @@
     <t>pre</t>
   </si>
   <si>
-    <t>reporth_g</t>
-  </si>
-  <si>
     <t>reporth_ICU</t>
   </si>
   <si>
@@ -2824,6 +2821,9 @@
   </si>
   <si>
     <t>(There is a limit to 50 interventions).</t>
+  </si>
+  <si>
+    <t>report_g</t>
   </si>
 </sst>
 </file>
@@ -3593,7 +3593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -3602,7 +3602,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21">
@@ -3627,32 +3627,32 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="59" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="34">
       <c r="A8" s="38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="17">
       <c r="A9" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="17">
       <c r="A10" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="17">
       <c r="A11" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="34">
       <c r="A12" s="38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -3667,7 +3667,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="85" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -3695,7 +3695,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="85" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -4117,7 +4117,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B19" s="7">
         <v>43983</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -4692,7 +4692,7 @@
         <v>147</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>103</v>
@@ -4706,7 +4706,7 @@
         <v>319</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -7192,8 +7192,8 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7229,7 +7229,7 @@
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="64" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B2" s="62">
         <v>43862</v>
@@ -7245,7 +7245,7 @@
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="64" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B3" s="62">
         <v>44196</v>
@@ -7261,7 +7261,7 @@
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" s="64" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="70">
@@ -7277,7 +7277,7 @@
     </row>
     <row r="5" spans="1:6" s="73" customFormat="1" ht="17">
       <c r="A5" s="64" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B5" s="69"/>
       <c r="C5" s="71">
@@ -7295,7 +7295,7 @@
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="64" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B6" s="61"/>
       <c r="C6" s="63">
@@ -7311,7 +7311,7 @@
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="64" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" s="61"/>
       <c r="C7" s="63">
@@ -7329,7 +7329,7 @@
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="64" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B8" s="61"/>
       <c r="C8" s="63">
@@ -7347,7 +7347,7 @@
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="64" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B9" s="61"/>
       <c r="C9" s="63">
@@ -7360,12 +7360,12 @@
         <v>47</v>
       </c>
       <c r="F9" s="67" t="s">
-        <v>378</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34">
       <c r="A10" s="64" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B10" s="61"/>
       <c r="C10" s="63">
@@ -7383,7 +7383,7 @@
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="64" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="63">
@@ -7396,12 +7396,12 @@
         <v>47</v>
       </c>
       <c r="F11" s="67" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34">
       <c r="A12" s="64" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B12" s="61"/>
       <c r="C12" s="63">
@@ -7414,12 +7414,12 @@
         <v>47</v>
       </c>
       <c r="F12" s="67" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34">
       <c r="A13" s="64" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B13" s="61"/>
       <c r="C13" s="63">
@@ -7432,12 +7432,12 @@
         <v>47</v>
       </c>
       <c r="F13" s="67" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34">
       <c r="A14" s="64" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B14" s="61"/>
       <c r="C14" s="63">
@@ -7450,12 +7450,12 @@
         <v>47</v>
       </c>
       <c r="F14" s="67" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34">
       <c r="A15" s="64" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B15" s="61"/>
       <c r="C15" s="63">
@@ -7468,12 +7468,12 @@
         <v>47</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34">
       <c r="A16" s="64" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B16" s="61"/>
       <c r="C16" s="63">
@@ -7486,12 +7486,12 @@
         <v>47</v>
       </c>
       <c r="F16" s="67" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34">
       <c r="A17" s="64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B17" s="61"/>
       <c r="C17" s="63">
@@ -7504,12 +7504,12 @@
         <v>47</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="64" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B18" s="61"/>
       <c r="C18" s="63">
@@ -7522,12 +7522,12 @@
         <v>47</v>
       </c>
       <c r="F18" s="67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34">
       <c r="A19" s="64" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B19" s="61"/>
       <c r="C19" s="63">
@@ -7540,12 +7540,12 @@
         <v>47</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34">
       <c r="A20" s="64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B20" s="61"/>
       <c r="C20" s="63">
@@ -7558,7 +7558,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
@@ -7693,7 +7693,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>277</v>
@@ -7709,7 +7709,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C3" s="1">
         <v>2.8</v>
@@ -7726,7 +7726,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -7808,7 +7808,7 @@
     </row>
     <row r="2" spans="1:5" ht="17">
       <c r="A2" s="75" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B2" s="77">
         <v>10</v>
@@ -7825,7 +7825,7 @@
     </row>
     <row r="3" spans="1:5" ht="17">
       <c r="A3" s="75" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B3" s="77">
         <v>3.5</v>
@@ -7842,7 +7842,7 @@
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="75" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B4" s="77">
         <v>4.5</v>
@@ -7859,7 +7859,7 @@
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="75" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B5" s="77">
         <v>1</v>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B6" s="77">
         <v>0</v>
@@ -7891,7 +7891,7 @@
     </row>
     <row r="7" spans="1:5" ht="17">
       <c r="A7" s="75" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B7" s="77">
         <v>150</v>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="75" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B8" s="77">
         <v>55</v>
@@ -7925,7 +7925,7 @@
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="75" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B9" s="77">
         <v>50</v>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="75" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B10" s="77">
         <v>75</v>
@@ -7976,7 +7976,7 @@
     </row>
     <row r="12" spans="1:5" ht="34">
       <c r="A12" s="75" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B12" s="79">
         <v>50</v>
@@ -7988,12 +7988,12 @@
         <v>47</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="34">
       <c r="A13" s="75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B13" s="79">
         <v>50</v>
@@ -8005,12 +8005,12 @@
         <v>47</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="34">
       <c r="A14" s="75" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B14" s="79">
         <v>50</v>
@@ -8022,12 +8022,12 @@
         <v>47</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34">
       <c r="A15" s="75" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B15" s="79">
         <v>50</v>
@@ -8039,12 +8039,12 @@
         <v>47</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="34">
       <c r="A16" s="75" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B16" s="79">
         <v>50</v>
@@ -8056,12 +8056,12 @@
         <v>47</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34">
       <c r="A17" s="75" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B17" s="79">
         <v>50</v>
@@ -8073,12 +8073,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
       <c r="A18" s="75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B18" s="79">
         <v>50</v>
@@ -8090,12 +8090,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
       <c r="A19" s="75" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B19" s="79">
         <v>50</v>
@@ -8107,12 +8107,12 @@
         <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A20" s="75" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B20" s="81">
         <v>50</v>
@@ -8124,12 +8124,12 @@
         <v>47</v>
       </c>
       <c r="E20" s="82" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A21" s="76" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B21" s="81">
         <v>0</v>
@@ -8141,12 +8141,12 @@
         <v>47</v>
       </c>
       <c r="E21" s="82" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="74" customFormat="1" ht="17" customHeight="1">
       <c r="A22" s="75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B22" s="81">
         <v>100</v>
@@ -8158,12 +8158,12 @@
         <v>47</v>
       </c>
       <c r="E22" s="82" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="74" customFormat="1" ht="17" customHeight="1">
       <c r="A23" s="75" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B23" s="81">
         <v>100</v>
@@ -8175,12 +8175,12 @@
         <v>47</v>
       </c>
       <c r="E23" s="82" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="74" customFormat="1" ht="34">
       <c r="A24" s="75" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B24" s="81">
         <v>100</v>
@@ -8192,12 +8192,12 @@
         <v>47</v>
       </c>
       <c r="E24" s="82" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="74" customFormat="1" ht="17">
       <c r="A25" s="75" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B25" s="81">
         <v>100</v>
@@ -8209,7 +8209,7 @@
         <v>47</v>
       </c>
       <c r="E25" s="82" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -8547,7 +8547,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B17">
         <v>95</v>
@@ -8559,12 +8559,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B18">
         <v>95</v>
@@ -8576,12 +8576,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B19">
         <v>95</v>
@@ -8593,7 +8593,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -9129,7 +9129,7 @@
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="53"/>
       <c r="B30" s="50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C30" s="41">
         <v>4</v>
@@ -9165,7 +9165,7 @@
     <row r="32" spans="1:6" ht="17">
       <c r="A32" s="53"/>
       <c r="B32" s="33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C32" s="11">
         <v>100</v>
@@ -9177,13 +9177,13 @@
         <v>47</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17">
       <c r="A33" s="53"/>
       <c r="B33" s="33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C33" s="11">
         <v>100</v>
@@ -9195,13 +9195,13 @@
         <v>47</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34">
       <c r="A34" s="53"/>
       <c r="B34" s="33" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C34" s="11">
         <v>100</v>
@@ -9213,13 +9213,13 @@
         <v>47</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17">
       <c r="A35" s="53"/>
       <c r="B35" s="33" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C35" s="83">
         <v>100</v>
@@ -9237,7 +9237,7 @@
     <row r="36" spans="1:6" ht="18" thickBot="1">
       <c r="A36" s="46"/>
       <c r="B36" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C36" s="29">
         <v>100</v>
@@ -9249,7 +9249,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -9383,7 +9383,7 @@
     <row r="45" spans="1:6" ht="34">
       <c r="A45" s="53"/>
       <c r="B45" s="51" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C45" s="56">
         <v>82</v>

</xml_diff>

<commit_message>
default end date set to 2021-06-30
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/CoMo/como/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC6C1E3-F773-684E-96DA-2A555A72F017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BF5F54-8EE5-5642-9D9C-88ACD7C7FA4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="460" windowWidth="26960" windowHeight="17540" tabRatio="648" activeTab="4" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
@@ -7193,7 +7193,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7248,7 +7248,7 @@
         <v>448</v>
       </c>
       <c r="B3" s="62">
-        <v>44196</v>
+        <v>44377</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
@@ -7612,7 +7612,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="8">
+  <dataValidations count="8">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{B93D921B-ACCD-B540-B62C-AE19092FA296}">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
@@ -8263,7 +8263,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
removed school_eff and travelban_eff
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App.xlsx
+++ b/Template_CoMoCOVID-19App.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7759E-9BC0-E041-AC0F-91E9BCA7C61A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3722C32D-C3B9-4047-B5BD-D392D5BAB35E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="24380" windowHeight="18380" tabRatio="648" firstSheet="1" activeTab="9" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" tabRatio="648" activeTab="8" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="HIDDEN" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Interventions Param'!$A$1:$F$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="503">
   <si>
     <t>0-5 y.o.</t>
   </si>
@@ -340,9 +340,6 @@
     <t>Home contacts inflation due to school closure:</t>
   </si>
   <si>
-    <t>school_eff</t>
-  </si>
-  <si>
     <t>s2h</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t>age_cocoon</t>
-  </si>
-  <si>
-    <t>travelban_eff</t>
   </si>
   <si>
     <t>quarantine_days</t>
@@ -2987,6 +2981,29 @@
   </si>
   <si>
     <t>1-21 &lt;=&gt; All population.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interventions Param sheet.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Removed school_eff and travelban_eff. Values of these two parameters are taken off the "Interventions" tab instead.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3238,7 +3255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3454,12 +3471,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3504,16 +3534,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3528,14 +3548,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="E1:F15" xr:uid="{2E89BE7F-E667-6946-928D-DC5AB4119A65}"/>
   <sortState ref="E2:F8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3838,10 +3858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E13D8F-D093-7849-84D5-273B640F7707}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3851,7 +3871,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="94" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21">
@@ -3876,12 +3896,12 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="58" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="89" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3889,93 +3909,93 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="93" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F15" s="39"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="93" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F16" s="39"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="93" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F17" s="39"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="93" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F18" s="39"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="93" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="93" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="93" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F21" s="39"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="93" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F22" s="39"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="93" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F23" s="39"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="93" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="93" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6" s="38" customFormat="1">
       <c r="A26" s="93" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B26"/>
       <c r="D26"/>
@@ -3983,149 +4003,166 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="93" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="93" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F28" s="39"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="93" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F29" s="39"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="93" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="93" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="93" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="93" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F33" s="39"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="93" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F34" s="39"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="93" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F35" s="39"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="86" t="s">
-        <v>500</v>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="34">
+      <c r="A38" s="95" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="89" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="34">
-      <c r="A40" s="37" t="s">
+      <c r="A39" s="86"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="86"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="86"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="86"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="89" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="34">
+      <c r="A45" s="37" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17">
+      <c r="A46" s="37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17">
+      <c r="A47" s="37" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17">
+      <c r="A48" s="37" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="34">
+      <c r="A49" s="37" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="83" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="39" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="84" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="34">
+      <c r="A56" s="37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="34">
+      <c r="A57" s="37" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="68">
+      <c r="A58" s="37" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="37"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="84" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17">
-      <c r="A41" s="37" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="17">
-      <c r="A42" s="37" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="17">
-      <c r="A43" s="37" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="34">
-      <c r="A44" s="37" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="83" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="39" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="84" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="34">
-      <c r="A51" s="37" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="34">
-      <c r="A52" s="37" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="68">
-      <c r="A53" s="37" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="37"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="84" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4140,7 +4177,7 @@
   </sheetPr>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -4158,13 +4195,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17">
       <c r="A1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>45</v>
@@ -4173,15 +4210,15 @@
         <v>54</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B2" s="6">
         <v>43876</v>
@@ -4198,12 +4235,12 @@
       </c>
       <c r="F2" s="91"/>
       <c r="G2" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="6">
         <v>43937</v>
@@ -4220,12 +4257,12 @@
       </c>
       <c r="F3" s="92"/>
       <c r="G3" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="6">
         <v>43876</v>
@@ -4242,12 +4279,12 @@
       </c>
       <c r="F4" s="92"/>
       <c r="G4" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B5" s="6">
         <v>43876</v>
@@ -4264,12 +4301,12 @@
       </c>
       <c r="F5" s="92"/>
       <c r="G5" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B6" s="6">
         <v>43876</v>
@@ -4286,7 +4323,7 @@
       </c>
       <c r="F6" s="92"/>
       <c r="G6" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4308,12 +4345,12 @@
       </c>
       <c r="F7" s="92"/>
       <c r="G7" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B8" s="6">
         <v>43937</v>
@@ -4330,12 +4367,12 @@
       </c>
       <c r="F8" s="92"/>
       <c r="G8" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="6">
         <v>43876</v>
@@ -4352,12 +4389,12 @@
       </c>
       <c r="F9" s="92"/>
       <c r="G9" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B10" s="6">
         <v>43876</v>
@@ -4374,12 +4411,12 @@
       </c>
       <c r="F10" s="92"/>
       <c r="G10" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B11" s="6">
         <v>43876</v>
@@ -4396,12 +4433,12 @@
       </c>
       <c r="F11" s="92"/>
       <c r="G11" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B12" s="6">
         <v>43876</v>
@@ -4418,7 +4455,7 @@
       </c>
       <c r="F12" s="92"/>
       <c r="G12" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4440,12 +4477,12 @@
       </c>
       <c r="F13" s="92"/>
       <c r="G13" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B14" s="6">
         <v>43891</v>
@@ -4461,10 +4498,10 @@
         <v>thousand tests</v>
       </c>
       <c r="F14" s="92" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4485,15 +4522,15 @@
         <v>%</v>
       </c>
       <c r="F15" s="92" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" s="6">
         <v>43910</v>
@@ -4510,12 +4547,12 @@
       </c>
       <c r="F16" s="92"/>
       <c r="G16" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="6">
         <v>43983</v>
@@ -4531,10 +4568,10 @@
         <v>%</v>
       </c>
       <c r="F17" s="92" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5547,7 +5584,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F101">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(OR($A2 = "Vaccination", $A2 = "School Closures",  $A2 = "Mass Testing"))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5597,19 +5634,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E1" s="90" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F1" s="90" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -5617,16 +5654,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -5634,7 +5671,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>87</v>
@@ -5643,15 +5680,15 @@
         <v>52</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="C4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>52</v>
@@ -5659,10 +5696,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="C5" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>52</v>
@@ -5670,18 +5707,18 @@
     </row>
     <row r="6" spans="1:9">
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>89</v>
@@ -5692,10 +5729,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="C8" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>52</v>
@@ -5703,10 +5740,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="C9" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>52</v>
@@ -5714,21 +5751,21 @@
     </row>
     <row r="10" spans="1:9">
       <c r="C10" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="C11" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>52</v>
@@ -5736,7 +5773,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="C12" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>86</v>
@@ -5747,10 +5784,10 @@
     </row>
     <row r="13" spans="1:9">
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>52</v>
@@ -5758,7 +5795,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="C14" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>88</v>
@@ -5769,700 +5806,700 @@
     </row>
     <row r="15" spans="1:9">
       <c r="C15" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="C16" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="3:3">
       <c r="C28" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="3:3">
       <c r="C59" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="3:3">
       <c r="C60" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="3:3">
       <c r="C71" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="3:3">
       <c r="C73" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="3:3">
       <c r="C78" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="3:3">
       <c r="C79" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" spans="3:3">
       <c r="C140" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="3:3">
       <c r="C141" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="3:3">
       <c r="C142" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="3:3">
       <c r="C143" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="3:3">
       <c r="C144" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="3:3">
       <c r="C147" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="3:3">
       <c r="C148" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" spans="3:3">
       <c r="C149" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" spans="3:3">
       <c r="C153" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -6490,13 +6527,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="68">
       <c r="A1" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -7633,13 +7670,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="170">
       <c r="A1" s="79" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -7905,16 +7942,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="68">
       <c r="A1" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8232,7 +8269,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8268,7 +8305,7 @@
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="63" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B2" s="61">
         <v>43862</v>
@@ -8276,15 +8313,15 @@
       <c r="C2" s="60"/>
       <c r="D2" s="60"/>
       <c r="E2" s="59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="A3" s="63" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B3" s="61">
         <v>44377</v>
@@ -8292,15 +8329,15 @@
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
       <c r="E3" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>127</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" s="63" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B4" s="68"/>
       <c r="C4" s="69">
@@ -8311,16 +8348,16 @@
         <v>44</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="72" customFormat="1" ht="17">
       <c r="A5" s="63" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B5" s="68"/>
       <c r="C5" s="70">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>52</v>
@@ -8329,12 +8366,12 @@
         <v>47</v>
       </c>
       <c r="F5" s="66" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="63" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="62">
@@ -8345,12 +8382,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="63" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B7" s="60"/>
       <c r="C7" s="62">
@@ -8363,12 +8400,12 @@
         <v>47</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="63" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="62">
@@ -8381,12 +8418,12 @@
         <v>47</v>
       </c>
       <c r="F8" s="59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="63" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B9" s="60"/>
       <c r="C9" s="62">
@@ -8399,12 +8436,12 @@
         <v>47</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34">
       <c r="A10" s="63" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B10" s="60"/>
       <c r="C10" s="62">
@@ -8417,12 +8454,12 @@
         <v>47</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="63" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B11" s="60"/>
       <c r="C11" s="62">
@@ -8435,12 +8472,12 @@
         <v>47</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34">
       <c r="A12" s="63" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B12" s="60"/>
       <c r="C12" s="62">
@@ -8453,12 +8490,12 @@
         <v>47</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34">
       <c r="A13" s="63" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B13" s="60"/>
       <c r="C13" s="62">
@@ -8471,12 +8508,12 @@
         <v>47</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34">
       <c r="A14" s="63" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="62">
@@ -8489,12 +8526,12 @@
         <v>47</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34">
       <c r="A15" s="63" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B15" s="60"/>
       <c r="C15" s="62">
@@ -8507,12 +8544,12 @@
         <v>47</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34">
       <c r="A16" s="63" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B16" s="60"/>
       <c r="C16" s="62">
@@ -8525,12 +8562,12 @@
         <v>47</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34">
       <c r="A17" s="63" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B17" s="60"/>
       <c r="C17" s="62">
@@ -8543,12 +8580,12 @@
         <v>47</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="63" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B18" s="60"/>
       <c r="C18" s="62">
@@ -8561,12 +8598,12 @@
         <v>47</v>
       </c>
       <c r="F18" s="66" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34">
       <c r="A19" s="63" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B19" s="60"/>
       <c r="C19" s="62">
@@ -8579,12 +8616,12 @@
         <v>47</v>
       </c>
       <c r="F19" s="66" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34">
       <c r="A20" s="63" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B20" s="60"/>
       <c r="C20" s="62">
@@ -8597,12 +8634,12 @@
         <v>47</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
       <c r="A21" s="71" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B21" s="64"/>
       <c r="C21" s="65">
@@ -8613,12 +8650,12 @@
         <v>47</v>
       </c>
       <c r="F21" s="66" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17">
       <c r="A22" s="71" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B22" s="64"/>
       <c r="C22" s="67">
@@ -8629,12 +8666,12 @@
         <v>47</v>
       </c>
       <c r="F22" s="66" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17">
       <c r="A23" s="71" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B23" s="64"/>
       <c r="C23" s="67">
@@ -8647,7 +8684,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="66" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -8715,7 +8752,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>45</v>
@@ -8732,23 +8769,23 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C3" s="1">
         <v>2.8</v>
@@ -8765,7 +8802,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -8847,7 +8884,7 @@
     </row>
     <row r="2" spans="1:5" ht="17">
       <c r="A2" s="74" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B2" s="76">
         <v>10</v>
@@ -8864,7 +8901,7 @@
     </row>
     <row r="3" spans="1:5" ht="17">
       <c r="A3" s="74" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B3" s="76">
         <v>3.5</v>
@@ -8881,7 +8918,7 @@
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="74" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B4" s="76">
         <v>4.5</v>
@@ -8898,7 +8935,7 @@
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="74" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B5" s="76">
         <v>1</v>
@@ -8913,7 +8950,7 @@
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="74" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B6" s="76">
         <v>0</v>
@@ -8930,7 +8967,7 @@
     </row>
     <row r="7" spans="1:5" ht="17">
       <c r="A7" s="74" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B7" s="76">
         <v>150</v>
@@ -8947,7 +8984,7 @@
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="74" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B8" s="76">
         <v>55</v>
@@ -8964,7 +9001,7 @@
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="74" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B9" s="76">
         <v>50</v>
@@ -8981,7 +9018,7 @@
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="74" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B10" s="76">
         <v>75</v>
@@ -8998,7 +9035,7 @@
     </row>
     <row r="11" spans="1:5" ht="17">
       <c r="A11" s="74" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B11" s="77">
         <v>50</v>
@@ -9010,12 +9047,12 @@
         <v>47</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="34">
       <c r="A12" s="74" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B12" s="78">
         <v>50</v>
@@ -9027,12 +9064,12 @@
         <v>47</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="34">
       <c r="A13" s="74" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B13" s="78">
         <v>50</v>
@@ -9044,12 +9081,12 @@
         <v>47</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="34">
       <c r="A14" s="74" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B14" s="78">
         <v>50</v>
@@ -9061,12 +9098,12 @@
         <v>47</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="34">
       <c r="A15" s="74" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B15" s="78">
         <v>50</v>
@@ -9078,12 +9115,12 @@
         <v>47</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="34">
       <c r="A16" s="74" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B16" s="78">
         <v>50</v>
@@ -9095,12 +9132,12 @@
         <v>47</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34">
       <c r="A17" s="74" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B17" s="78">
         <v>50</v>
@@ -9112,12 +9149,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34">
       <c r="A18" s="74" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B18" s="78">
         <v>50</v>
@@ -9129,12 +9166,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
       <c r="A19" s="74" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B19" s="78">
         <v>50</v>
@@ -9146,12 +9183,12 @@
         <v>47</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="73" customFormat="1" ht="34">
       <c r="A20" s="74" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B20" s="80">
         <v>50</v>
@@ -9163,12 +9200,12 @@
         <v>47</v>
       </c>
       <c r="E20" s="81" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="73" customFormat="1" ht="34">
       <c r="A21" s="75" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B21" s="80">
         <v>0</v>
@@ -9180,12 +9217,12 @@
         <v>47</v>
       </c>
       <c r="E21" s="81" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="73" customFormat="1" ht="17" customHeight="1">
       <c r="A22" s="74" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B22" s="80">
         <v>100</v>
@@ -9197,12 +9234,12 @@
         <v>47</v>
       </c>
       <c r="E22" s="81" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="73" customFormat="1" ht="17" customHeight="1">
       <c r="A23" s="74" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B23" s="80">
         <v>100</v>
@@ -9214,12 +9251,12 @@
         <v>47</v>
       </c>
       <c r="E23" s="81" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="73" customFormat="1" ht="34">
       <c r="A24" s="74" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B24" s="80">
         <v>100</v>
@@ -9231,12 +9268,12 @@
         <v>47</v>
       </c>
       <c r="E24" s="81" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="73" customFormat="1" ht="17">
       <c r="A25" s="74" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B25" s="80">
         <v>100</v>
@@ -9248,7 +9285,7 @@
         <v>47</v>
       </c>
       <c r="E25" s="81" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -9334,7 +9371,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B2" s="36">
         <v>160000</v>
@@ -9351,7 +9388,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" s="36">
         <v>8000</v>
@@ -9368,7 +9405,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="36">
         <v>8000</v>
@@ -9385,7 +9422,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -9402,7 +9439,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -9411,12 +9448,12 @@
         <v>47</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B7" s="5">
         <v>35</v>
@@ -9433,7 +9470,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B8" s="5">
         <v>35</v>
@@ -9445,12 +9482,12 @@
         <v>47</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B9" s="5">
         <v>50</v>
@@ -9467,7 +9504,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B10" s="5">
         <v>50</v>
@@ -9479,12 +9516,12 @@
         <v>47</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B11" s="5">
         <v>55</v>
@@ -9501,7 +9538,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B12" s="5">
         <v>55</v>
@@ -9513,12 +9550,12 @@
         <v>47</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B13" s="5">
         <v>75</v>
@@ -9535,7 +9572,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B14" s="5">
         <v>75</v>
@@ -9547,7 +9584,7 @@
         <v>47</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -9586,7 +9623,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B17">
         <v>95</v>
@@ -9598,12 +9635,12 @@
         <v>47</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B18">
         <v>95</v>
@@ -9615,12 +9652,12 @@
         <v>47</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B19">
         <v>95</v>
@@ -9632,12 +9669,12 @@
         <v>47</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
@@ -9654,7 +9691,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
@@ -9671,7 +9708,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -9716,9 +9753,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
@@ -9753,7 +9792,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
@@ -9781,7 +9820,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="26"/>
@@ -9792,7 +9831,7 @@
     <row r="5" spans="1:6" ht="17">
       <c r="A5" s="17"/>
       <c r="B5" s="34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C5" s="27">
         <v>4</v>
@@ -9802,13 +9841,13 @@
         <v>47</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" thickBot="1">
       <c r="A6" s="17"/>
       <c r="B6" s="34" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C6" s="27">
         <v>80</v>
@@ -9820,12 +9859,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="26"/>
@@ -9836,7 +9875,7 @@
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="14"/>
       <c r="B8" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" s="10">
         <v>14</v>
@@ -9848,13 +9887,13 @@
         <v>47</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34">
       <c r="A9" s="14"/>
       <c r="B9" s="34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C9" s="27">
         <v>2</v>
@@ -9866,13 +9905,13 @@
         <v>47</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34">
       <c r="A10" s="14"/>
       <c r="B10" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="10">
         <v>20</v>
@@ -9884,13 +9923,13 @@
         <v>47</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="35" thickBot="1">
       <c r="A11" s="20"/>
       <c r="B11" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="28">
         <v>100</v>
@@ -9902,7 +9941,7 @@
         <v>47</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -9946,7 +9985,7 @@
     <row r="15" spans="1:6" ht="18" thickBot="1">
       <c r="A15" s="45"/>
       <c r="B15" s="49" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C15" s="47">
         <v>20</v>
@@ -9958,12 +9997,12 @@
         <v>47</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="41" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="43"/>
@@ -9974,7 +10013,7 @@
     <row r="17" spans="1:6" ht="18" thickBot="1">
       <c r="A17" s="45"/>
       <c r="B17" s="50" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C17" s="51">
         <v>15</v>
@@ -9986,7 +10025,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -10045,432 +10084,386 @@
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:6" ht="17">
-      <c r="A22" s="52"/>
-      <c r="B22" s="49" t="s">
+    <row r="22" spans="1:6" ht="18" thickBot="1">
+      <c r="A22" s="45"/>
+      <c r="B22" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="47">
+        <v>20</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="1:6" ht="17">
+      <c r="A24" s="52"/>
+      <c r="B24" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="40">
-        <v>85</v>
-      </c>
-      <c r="D22" s="53" t="s">
+      <c r="C24" s="40">
+        <v>95</v>
+      </c>
+      <c r="D24" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E24" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F24" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18" thickBot="1">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25" s="47">
+        <v>70</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:6" ht="17">
+      <c r="A27" s="52"/>
+      <c r="B27" s="49" t="s">
+        <v>446</v>
+      </c>
+      <c r="C27" s="40">
+        <v>4</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17">
+      <c r="A28" s="52"/>
+      <c r="B28" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="C28" s="40">
+        <v>10</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17">
+      <c r="A29" s="52"/>
+      <c r="B29" s="32" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="18" thickBot="1">
-      <c r="A23" s="45"/>
-      <c r="B23" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="47">
-        <v>20</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="18" t="s">
+      <c r="D29" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:6" ht="17">
-      <c r="A25" s="52"/>
-      <c r="B25" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="40">
-        <v>95</v>
-      </c>
-      <c r="D25" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18" thickBot="1">
-      <c r="A26" s="45"/>
-      <c r="B26" s="46" t="s">
-        <v>313</v>
-      </c>
-      <c r="C26" s="47">
-        <v>70</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="41" t="s">
-        <v>299</v>
-      </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:6" ht="18" thickBot="1">
-      <c r="A28" s="45"/>
-      <c r="B28" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="47">
-        <v>50</v>
-      </c>
-      <c r="D28" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="25"/>
+      <c r="F29" s="16" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="52"/>
-      <c r="B30" s="49" t="s">
-        <v>448</v>
-      </c>
-      <c r="C30" s="40">
-        <v>4</v>
-      </c>
-      <c r="D30" s="53" t="s">
-        <v>91</v>
+      <c r="B30" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="C30" s="10">
+        <v>100</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>61</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="34">
       <c r="A31" s="52"/>
-      <c r="B31" s="49" t="s">
-        <v>331</v>
-      </c>
-      <c r="C31" s="40">
-        <v>10</v>
-      </c>
-      <c r="D31" s="53" t="s">
+      <c r="B31" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="C31" s="10">
+        <v>100</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>318</v>
+        <v>449</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17">
       <c r="A32" s="52"/>
       <c r="B32" s="32" t="s">
-        <v>455</v>
-      </c>
-      <c r="C32" s="10">
+        <v>454</v>
+      </c>
+      <c r="C32" s="82">
         <v>100</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="17">
-      <c r="A33" s="52"/>
-      <c r="B33" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="C33" s="10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18" thickBot="1">
+      <c r="A33" s="45"/>
+      <c r="B33" s="35" t="s">
+        <v>455</v>
+      </c>
+      <c r="C33" s="28">
         <v>100</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="15" t="s">
+      <c r="D33" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="19" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="34">
-      <c r="A34" s="52"/>
-      <c r="B34" s="32" t="s">
-        <v>453</v>
-      </c>
-      <c r="C34" s="10">
-        <v>100</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>451</v>
-      </c>
+    <row r="34" spans="1:6">
+      <c r="A34" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="B34" s="42"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="25"/>
     </row>
     <row r="35" spans="1:6" ht="17">
       <c r="A35" s="52"/>
-      <c r="B35" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="C35" s="82">
-        <v>100</v>
-      </c>
-      <c r="D35" s="29" t="s">
+      <c r="B35" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="40">
+        <v>80</v>
+      </c>
+      <c r="D35" s="53" t="s">
         <v>52</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="18" thickBot="1">
-      <c r="A36" s="45"/>
-      <c r="B36" s="35" t="s">
-        <v>457</v>
-      </c>
-      <c r="C36" s="28">
-        <v>100</v>
-      </c>
-      <c r="D36" s="31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17">
+      <c r="A36" s="52"/>
+      <c r="B36" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" s="40">
+        <v>14</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17">
+      <c r="A37" s="52"/>
+      <c r="B37" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="C37" s="54">
+        <v>20</v>
+      </c>
+      <c r="D37" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18" thickBot="1">
+      <c r="A38" s="45"/>
+      <c r="B38" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="C38" s="47">
+        <v>60</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:6" ht="34">
+      <c r="A40" s="52"/>
+      <c r="B40" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="C40" s="55">
+        <v>82</v>
+      </c>
+      <c r="D40" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E40" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="41" t="s">
-        <v>319</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="25"/>
-    </row>
-    <row r="38" spans="1:6" ht="17">
-      <c r="A38" s="52"/>
-      <c r="B38" s="49" t="s">
-        <v>325</v>
-      </c>
-      <c r="C38" s="40">
-        <v>80</v>
-      </c>
-      <c r="D38" s="53" t="s">
+      <c r="F40" s="16" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="34">
+      <c r="A41" s="12"/>
+      <c r="B41" s="50" t="s">
+        <v>350</v>
+      </c>
+      <c r="C41" s="55">
+        <v>64</v>
+      </c>
+      <c r="D41" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E41" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="17">
-      <c r="A39" s="52"/>
-      <c r="B39" s="49" t="s">
-        <v>324</v>
-      </c>
-      <c r="C39" s="40">
-        <v>14</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="15" t="s">
+      <c r="F41" s="16" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="34">
+      <c r="A42" s="52"/>
+      <c r="B42" s="50" t="s">
+        <v>467</v>
+      </c>
+      <c r="C42" s="55">
+        <v>82</v>
+      </c>
+      <c r="D42" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17">
-      <c r="A40" s="52"/>
-      <c r="B40" s="49" t="s">
-        <v>326</v>
-      </c>
-      <c r="C40" s="54">
-        <v>20</v>
-      </c>
-      <c r="D40" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="15" t="s">
+      <c r="F42" s="16" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="34">
+      <c r="A43" s="52"/>
+      <c r="B43" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="C43" s="57">
+        <v>64</v>
+      </c>
+      <c r="D43" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="16" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="18" thickBot="1">
-      <c r="A41" s="45"/>
-      <c r="B41" s="46" t="s">
-        <v>327</v>
-      </c>
-      <c r="C41" s="47">
-        <v>60</v>
-      </c>
-      <c r="D41" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="F43" s="16" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18" thickBot="1">
+      <c r="A44" s="45"/>
+      <c r="B44" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="C44" s="51">
+        <v>87</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="41" t="s">
-        <v>349</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="25"/>
-    </row>
-    <row r="43" spans="1:6" ht="17">
-      <c r="A43" s="52"/>
-      <c r="B43" s="50" t="s">
-        <v>350</v>
-      </c>
-      <c r="C43" s="55">
-        <v>82</v>
-      </c>
-      <c r="D43" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="34">
-      <c r="A44" s="12"/>
-      <c r="B44" s="50" t="s">
-        <v>352</v>
-      </c>
-      <c r="C44" s="55">
-        <v>64</v>
-      </c>
-      <c r="D44" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="34">
-      <c r="A45" s="52"/>
-      <c r="B45" s="50" t="s">
-        <v>469</v>
-      </c>
-      <c r="C45" s="55">
-        <v>82</v>
-      </c>
-      <c r="D45" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="34">
-      <c r="A46" s="52"/>
-      <c r="B46" s="49" t="s">
-        <v>355</v>
-      </c>
-      <c r="C46" s="57">
-        <v>64</v>
-      </c>
-      <c r="D46" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="16" t="s">
+      <c r="F44" s="19" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="18" thickBot="1">
-      <c r="A47" s="45"/>
-      <c r="B47" s="46" t="s">
-        <v>357</v>
-      </c>
-      <c r="C47" s="51">
-        <v>87</v>
-      </c>
-      <c r="D47" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -10479,11 +10472,11 @@
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30" xr:uid="{79437B14-BBCB-41C8-B199-9D1512AD30EC}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27" xr:uid="{79437B14-BBCB-41C8-B199-9D1512AD30EC}">
       <formula1>1</formula1>
       <formula2>52</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C22:C23 C28 C10:C11 C38:C41 C25:C26 C19:C20 C13 C35:C36" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C10:C11 C35:C38 C24:C25 C19:C20 C13 C32:C33 C22" xr:uid="{0227A7DA-52BF-41F5-B1CC-7112D8A0D503}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -10507,7 +10500,7 @@
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43:C47 C31:C32" xr:uid="{B3A77258-E555-9644-BB0D-41361904BE89}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C44 C28:C29" xr:uid="{B3A77258-E555-9644-BB0D-41361904BE89}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -10515,7 +10508,7 @@
       <formula1>0</formula1>
       <formula2>35</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C34" xr:uid="{7677C1D3-EA04-914A-8C0E-39F794492804}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:C31" xr:uid="{7677C1D3-EA04-914A-8C0E-39F794492804}">
       <formula1>0.08</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>